<commit_message>
inclusão alterações documento oficial excel
</commit_message>
<xml_diff>
--- a/API/documentos/Dados Entrada Cliente.xlsx
+++ b/API/documentos/Dados Entrada Cliente.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Geração propriedades" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7630" uniqueCount="1115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7728" uniqueCount="1117">
   <si>
     <t>tb_pes</t>
   </si>
@@ -3371,7 +3371,13 @@
     <t>registroDocumento</t>
   </si>
   <si>
+    <t>registroVinculo</t>
+  </si>
+  <si>
     <t>registroReferencia</t>
+  </si>
+  <si>
+    <t>registroPessoaSimplificada</t>
   </si>
 </sst>
 </file>
@@ -3803,8 +3809,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G362"/>
   <sheetViews>
-    <sheetView topLeftCell="A144" workbookViewId="0">
-      <selection activeCell="A168" sqref="A168"/>
+    <sheetView tabSelected="1" topLeftCell="A310" workbookViewId="0">
+      <selection activeCell="G362" activeCellId="1" sqref="G352:G358 G362"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6791,19 +6797,20 @@
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
-        <v>0</v>
-      </c>
-      <c r="B129" t="s">
+      <c r="A129" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B129" s="21" t="s">
         <v>1057</v>
       </c>
-      <c r="C129" s="2" t="s">
+      <c r="C129" s="21" t="s">
         <v>211</v>
       </c>
-      <c r="E129" t="s">
+      <c r="D129" s="21"/>
+      <c r="E129" s="21" t="s">
         <v>1058</v>
       </c>
-      <c r="F129" t="s">
+      <c r="F129" s="21" t="s">
         <v>3</v>
       </c>
       <c r="G129" t="str">
@@ -7295,19 +7302,20 @@
       </c>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A153" t="s">
-        <v>0</v>
-      </c>
-      <c r="B153" t="s">
+      <c r="A153" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B153" s="21" t="s">
         <v>1035</v>
       </c>
-      <c r="C153" t="s">
+      <c r="C153" s="21" t="s">
         <v>235</v>
       </c>
-      <c r="E153" t="s">
+      <c r="D153" s="21"/>
+      <c r="E153" s="21" t="s">
         <v>1036</v>
       </c>
-      <c r="F153" t="s">
+      <c r="F153" s="21" t="s">
         <v>3</v>
       </c>
       <c r="G153" t="str">
@@ -7316,22 +7324,22 @@
       </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A154" t="s">
-        <v>0</v>
-      </c>
-      <c r="B154" t="s">
+      <c r="A154" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B154" s="21" t="s">
         <v>236</v>
       </c>
-      <c r="C154" t="s">
+      <c r="C154" s="21" t="s">
         <v>236</v>
       </c>
-      <c r="D154" t="s">
+      <c r="D154" s="21" t="s">
         <v>237</v>
       </c>
-      <c r="E154" t="s">
+      <c r="E154" s="21" t="s">
         <v>744</v>
       </c>
-      <c r="F154" t="s">
+      <c r="F154" s="21" t="s">
         <v>3</v>
       </c>
       <c r="G154" t="str">
@@ -7340,22 +7348,22 @@
       </c>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A155" t="s">
-        <v>0</v>
-      </c>
-      <c r="B155" t="s">
+      <c r="A155" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B155" s="21" t="s">
         <v>238</v>
       </c>
-      <c r="C155" t="s">
+      <c r="C155" s="21" t="s">
         <v>238</v>
       </c>
-      <c r="D155" t="s">
+      <c r="D155" s="21" t="s">
         <v>239</v>
       </c>
-      <c r="E155" t="s">
+      <c r="E155" s="21" t="s">
         <v>745</v>
       </c>
-      <c r="F155" t="s">
+      <c r="F155" s="21" t="s">
         <v>3</v>
       </c>
       <c r="G155" t="str">
@@ -10794,19 +10802,20 @@
       </c>
     </row>
     <row r="318" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A318" t="s">
+      <c r="A318" s="21" t="s">
         <v>517</v>
       </c>
-      <c r="B318" t="s">
+      <c r="B318" s="21" t="s">
         <v>564</v>
       </c>
-      <c r="C318" s="10" t="s">
+      <c r="C318" s="21" t="s">
         <v>915</v>
       </c>
-      <c r="E318" t="s">
+      <c r="D318" s="21"/>
+      <c r="E318" s="21" t="s">
         <v>915</v>
       </c>
-      <c r="F318" t="s">
+      <c r="F318" s="21" t="s">
         <v>3</v>
       </c>
       <c r="G318" t="str">
@@ -10815,19 +10824,20 @@
       </c>
     </row>
     <row r="319" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A319" s="2" t="s">
+      <c r="A319" s="21" t="s">
         <v>517</v>
       </c>
-      <c r="B319" s="2" t="s">
+      <c r="B319" s="21" t="s">
         <v>241</v>
       </c>
-      <c r="C319" s="11" t="s">
+      <c r="C319" s="21" t="s">
         <v>1084</v>
       </c>
-      <c r="E319" s="2" t="s">
+      <c r="D319" s="21"/>
+      <c r="E319" s="21" t="s">
         <v>1084</v>
       </c>
-      <c r="F319" s="2" t="s">
+      <c r="F319" s="21" t="s">
         <v>3</v>
       </c>
       <c r="G319" t="str">
@@ -10836,19 +10846,20 @@
       </c>
     </row>
     <row r="320" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A320" t="s">
+      <c r="A320" s="21" t="s">
         <v>517</v>
       </c>
-      <c r="B320" t="s">
+      <c r="B320" s="21" t="s">
         <v>242</v>
       </c>
-      <c r="C320" s="10" t="s">
+      <c r="C320" s="21" t="s">
         <v>861</v>
       </c>
-      <c r="E320" t="s">
+      <c r="D320" s="21"/>
+      <c r="E320" s="21" t="s">
         <v>1086</v>
       </c>
-      <c r="F320" t="s">
+      <c r="F320" s="21" t="s">
         <v>3</v>
       </c>
       <c r="G320" t="str">
@@ -11530,20 +11541,20 @@
       </c>
     </row>
     <row r="352" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A352" s="14" t="s">
+      <c r="A352" s="21" t="s">
         <v>361</v>
       </c>
-      <c r="B352" s="14"/>
-      <c r="C352" s="14" t="s">
+      <c r="B352" s="21"/>
+      <c r="C352" s="21" t="s">
         <v>960</v>
       </c>
-      <c r="D352" s="16" t="s">
+      <c r="D352" s="21" t="s">
         <v>394</v>
       </c>
-      <c r="E352" s="14" t="s">
+      <c r="E352" s="21" t="s">
         <v>960</v>
       </c>
-      <c r="F352" s="18" t="s">
+      <c r="F352" s="21" t="s">
         <v>3</v>
       </c>
       <c r="G352" s="14" t="str">
@@ -11552,20 +11563,20 @@
       </c>
     </row>
     <row r="353" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A353" s="14" t="s">
+      <c r="A353" s="21" t="s">
         <v>361</v>
       </c>
-      <c r="B353" s="14"/>
-      <c r="C353" s="14" t="s">
+      <c r="B353" s="21"/>
+      <c r="C353" s="21" t="s">
         <v>806</v>
       </c>
-      <c r="D353" s="16" t="s">
+      <c r="D353" s="21" t="s">
         <v>396</v>
       </c>
-      <c r="E353" s="14" t="s">
+      <c r="E353" s="21" t="s">
         <v>806</v>
       </c>
-      <c r="F353" s="18" t="s">
+      <c r="F353" s="21" t="s">
         <v>3</v>
       </c>
       <c r="G353" s="14" t="str">
@@ -11574,20 +11585,20 @@
       </c>
     </row>
     <row r="354" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A354" s="14" t="s">
+      <c r="A354" s="21" t="s">
         <v>361</v>
       </c>
-      <c r="B354" s="14"/>
-      <c r="C354" s="14" t="s">
+      <c r="B354" s="21"/>
+      <c r="C354" s="21" t="s">
         <v>808</v>
       </c>
-      <c r="D354" s="16" t="s">
+      <c r="D354" s="21" t="s">
         <v>398</v>
       </c>
-      <c r="E354" s="14" t="s">
+      <c r="E354" s="21" t="s">
         <v>808</v>
       </c>
-      <c r="F354" s="18" t="s">
+      <c r="F354" s="21" t="s">
         <v>3</v>
       </c>
       <c r="G354" s="14" t="str">
@@ -11596,20 +11607,20 @@
       </c>
     </row>
     <row r="355" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A355" s="14" t="s">
+      <c r="A355" s="21" t="s">
         <v>361</v>
       </c>
-      <c r="B355" s="14"/>
-      <c r="C355" s="14" t="s">
+      <c r="B355" s="21"/>
+      <c r="C355" s="21" t="s">
         <v>809</v>
       </c>
-      <c r="D355" s="16" t="s">
+      <c r="D355" s="21" t="s">
         <v>400</v>
       </c>
-      <c r="E355" s="14" t="s">
+      <c r="E355" s="21" t="s">
         <v>809</v>
       </c>
-      <c r="F355" s="18" t="s">
+      <c r="F355" s="21" t="s">
         <v>3</v>
       </c>
       <c r="G355" s="14" t="str">
@@ -11618,20 +11629,20 @@
       </c>
     </row>
     <row r="356" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A356" s="14" t="s">
+      <c r="A356" s="21" t="s">
         <v>361</v>
       </c>
-      <c r="B356" s="14"/>
-      <c r="C356" s="14" t="s">
+      <c r="B356" s="21"/>
+      <c r="C356" s="21" t="s">
         <v>810</v>
       </c>
-      <c r="D356" s="16" t="s">
+      <c r="D356" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="E356" s="14" t="s">
+      <c r="E356" s="21" t="s">
         <v>810</v>
       </c>
-      <c r="F356" s="18" t="s">
+      <c r="F356" s="21" t="s">
         <v>3</v>
       </c>
       <c r="G356" s="14" t="str">
@@ -11640,20 +11651,20 @@
       </c>
     </row>
     <row r="357" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A357" s="14" t="s">
+      <c r="A357" s="21" t="s">
         <v>361</v>
       </c>
-      <c r="B357" s="14"/>
-      <c r="C357" s="14" t="s">
+      <c r="B357" s="21"/>
+      <c r="C357" s="21" t="s">
         <v>811</v>
       </c>
-      <c r="D357" s="16" t="s">
+      <c r="D357" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="E357" s="14" t="s">
+      <c r="E357" s="21" t="s">
         <v>811</v>
       </c>
-      <c r="F357" s="18" t="s">
+      <c r="F357" s="21" t="s">
         <v>3</v>
       </c>
       <c r="G357" s="14" t="str">
@@ -11662,20 +11673,20 @@
       </c>
     </row>
     <row r="358" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A358" s="14" t="s">
+      <c r="A358" s="21" t="s">
         <v>361</v>
       </c>
-      <c r="B358" s="14"/>
-      <c r="C358" s="14" t="s">
+      <c r="B358" s="21"/>
+      <c r="C358" s="21" t="s">
         <v>812</v>
       </c>
-      <c r="D358" s="16" t="s">
+      <c r="D358" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="E358" s="14" t="s">
+      <c r="E358" s="21" t="s">
         <v>812</v>
       </c>
-      <c r="F358" s="18" t="s">
+      <c r="F358" s="21" t="s">
         <v>3</v>
       </c>
       <c r="G358" s="14" t="str">
@@ -11750,18 +11761,18 @@
       </c>
     </row>
     <row r="362" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A362" s="14" t="s">
+      <c r="A362" s="21" t="s">
         <v>361</v>
       </c>
-      <c r="B362" s="14"/>
-      <c r="C362" s="14" t="s">
+      <c r="B362" s="21"/>
+      <c r="C362" s="21" t="s">
         <v>816</v>
       </c>
-      <c r="D362" s="16"/>
-      <c r="E362" s="14" t="s">
+      <c r="D362" s="21"/>
+      <c r="E362" s="21" t="s">
         <v>816</v>
       </c>
-      <c r="F362" s="18" t="s">
+      <c r="F362" s="21" t="s">
         <v>3</v>
       </c>
       <c r="G362" s="14" t="str">
@@ -11779,8 +11790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J362"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
-      <selection activeCell="E153" sqref="E153"/>
+    <sheetView topLeftCell="A125" workbookViewId="0">
+      <selection activeCell="B153" sqref="B153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20070,7 +20081,7 @@
         <v>3</v>
       </c>
       <c r="G244" s="18" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
       <c r="H244" s="18" t="str">
         <f t="shared" si="12"/>
@@ -20103,7 +20114,7 @@
         <v>3</v>
       </c>
       <c r="G245" s="18" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
       <c r="H245" s="18" t="str">
         <f t="shared" si="12"/>
@@ -20136,7 +20147,7 @@
         <v>993</v>
       </c>
       <c r="G246" s="18" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
       <c r="H246" s="18" t="str">
         <f t="shared" si="12"/>
@@ -20169,7 +20180,7 @@
         <v>3</v>
       </c>
       <c r="G247" s="18" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
       <c r="H247" s="18" t="str">
         <f t="shared" si="12"/>
@@ -20202,7 +20213,7 @@
         <v>3</v>
       </c>
       <c r="G248" s="18" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
       <c r="H248" s="18" t="str">
         <f t="shared" si="12"/>
@@ -20235,7 +20246,7 @@
         <v>991</v>
       </c>
       <c r="G249" s="18" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
       <c r="H249" s="18" t="str">
         <f t="shared" si="12"/>
@@ -20268,7 +20279,7 @@
         <v>991</v>
       </c>
       <c r="G250" s="18" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
       <c r="H250" s="18" t="str">
         <f t="shared" si="12"/>
@@ -20301,7 +20312,7 @@
         <v>1089</v>
       </c>
       <c r="G251" s="18" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
       <c r="H251" s="18" t="str">
         <f t="shared" si="12"/>
@@ -20334,7 +20345,7 @@
         <v>1089</v>
       </c>
       <c r="G252" s="18" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
       <c r="H252" s="18" t="str">
         <f t="shared" si="12"/>
@@ -20367,7 +20378,7 @@
         <v>1089</v>
       </c>
       <c r="G253" s="18" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
       <c r="H253" s="18" t="str">
         <f t="shared" si="12"/>
@@ -20400,7 +20411,7 @@
         <v>3</v>
       </c>
       <c r="G254" s="18" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
       <c r="H254" s="18" t="str">
         <f t="shared" si="12"/>
@@ -20433,7 +20444,7 @@
         <v>1089</v>
       </c>
       <c r="G255" s="18" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
       <c r="H255" s="18" t="str">
         <f t="shared" si="12"/>
@@ -20466,7 +20477,7 @@
         <v>3</v>
       </c>
       <c r="G256" s="18" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
       <c r="H256" s="18" t="str">
         <f t="shared" si="12"/>
@@ -20499,7 +20510,7 @@
         <v>1089</v>
       </c>
       <c r="G257" s="18" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
       <c r="H257" s="18" t="str">
         <f t="shared" si="12"/>
@@ -20532,7 +20543,7 @@
         <v>993</v>
       </c>
       <c r="G258" s="18" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
       <c r="H258" s="18" t="str">
         <f t="shared" si="12"/>
@@ -20565,7 +20576,7 @@
         <v>993</v>
       </c>
       <c r="G259" s="18" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
       <c r="H259" s="18" t="str">
         <f t="shared" si="12"/>
@@ -20598,7 +20609,7 @@
         <v>3</v>
       </c>
       <c r="G260" s="18" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
       <c r="H260" s="18" t="str">
         <f t="shared" si="12"/>
@@ -20631,7 +20642,7 @@
         <v>3</v>
       </c>
       <c r="G261" s="18" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
       <c r="H261" s="18" t="str">
         <f t="shared" si="12"/>
@@ -20664,7 +20675,7 @@
         <v>3</v>
       </c>
       <c r="G262" s="18" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
       <c r="H262" s="18" t="str">
         <f t="shared" si="12"/>
@@ -20697,7 +20708,7 @@
         <v>1089</v>
       </c>
       <c r="G263" s="18" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
       <c r="H263" s="18" t="str">
         <f t="shared" si="12"/>
@@ -20743,6 +20754,9 @@
       <c r="F265" s="22" t="s">
         <v>3</v>
       </c>
+      <c r="G265" s="22" t="s">
+        <v>1116</v>
+      </c>
       <c r="H265" s="18" t="str">
         <f t="shared" si="12"/>
         <v>public string cod_simp  { get; set; }</v>
@@ -20753,7 +20767,7 @@
       </c>
       <c r="J265" s="18" t="str">
         <f t="shared" si="14"/>
-        <v>|if(!string.IsNullOrWhiteSpace(msg.codigo))| .cod_simp = msg.codigo;</v>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.codigo))| registroPessoaSimplificada.cod_simp = msg.codigo;</v>
       </c>
     </row>
     <row r="266" spans="1:10" x14ac:dyDescent="0.25">
@@ -20773,6 +20787,9 @@
       <c r="F266" s="22" t="s">
         <v>3</v>
       </c>
+      <c r="G266" s="22" t="s">
+        <v>1116</v>
+      </c>
       <c r="H266" s="18" t="str">
         <f t="shared" si="12"/>
         <v>public string nom_simp  { get; set; }</v>
@@ -20783,7 +20800,7 @@
       </c>
       <c r="J266" s="18" t="str">
         <f t="shared" si="14"/>
-        <v>|if(!string.IsNullOrWhiteSpace(msg.nome))| .nom_simp = msg.nome;</v>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.nome))| registroPessoaSimplificada.nom_simp = msg.nome;</v>
       </c>
     </row>
     <row r="267" spans="1:10" x14ac:dyDescent="0.25">
@@ -20803,6 +20820,9 @@
       <c r="F267" s="22" t="s">
         <v>3</v>
       </c>
+      <c r="G267" s="22" t="s">
+        <v>1116</v>
+      </c>
       <c r="H267" s="18" t="str">
         <f t="shared" si="12"/>
         <v>public string ddd_fone_1_simp  { get; set; }</v>
@@ -20813,7 +20833,7 @@
       </c>
       <c r="J267" s="18" t="str">
         <f t="shared" si="14"/>
-        <v>|if(!string.IsNullOrWhiteSpace(msg.codigoDddFone1))| .ddd_fone_1_simp = msg.codigoDddFone1;</v>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.codigoDddFone1))| registroPessoaSimplificada.ddd_fone_1_simp = msg.codigoDddFone1;</v>
       </c>
     </row>
     <row r="268" spans="1:10" x14ac:dyDescent="0.25">
@@ -20833,6 +20853,9 @@
       <c r="F268" s="22" t="s">
         <v>3</v>
       </c>
+      <c r="G268" s="22" t="s">
+        <v>1116</v>
+      </c>
       <c r="H268" s="18" t="str">
         <f t="shared" si="12"/>
         <v>public string ddd_fone_2_simp  { get; set; }</v>
@@ -20843,7 +20866,7 @@
       </c>
       <c r="J268" s="18" t="str">
         <f t="shared" si="14"/>
-        <v>|if(!string.IsNullOrWhiteSpace(msg.codigoDddFone2))| .ddd_fone_2_simp = msg.codigoDddFone2;</v>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.codigoDddFone2))| registroPessoaSimplificada.ddd_fone_2_simp = msg.codigoDddFone2;</v>
       </c>
     </row>
     <row r="269" spans="1:10" x14ac:dyDescent="0.25">
@@ -20863,6 +20886,9 @@
       <c r="F269" s="22" t="s">
         <v>3</v>
       </c>
+      <c r="G269" s="22" t="s">
+        <v>1116</v>
+      </c>
       <c r="H269" s="18" t="str">
         <f t="shared" si="12"/>
         <v>public string fone_1_simp  { get; set; }</v>
@@ -20873,7 +20899,7 @@
       </c>
       <c r="J269" s="18" t="str">
         <f t="shared" si="14"/>
-        <v>|if(!string.IsNullOrWhiteSpace(msg.numeroTelefone1))| .fone_1_simp = msg.numeroTelefone1;</v>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.numeroTelefone1))| registroPessoaSimplificada.fone_1_simp = msg.numeroTelefone1;</v>
       </c>
     </row>
     <row r="270" spans="1:10" x14ac:dyDescent="0.25">
@@ -20893,6 +20919,9 @@
       <c r="F270" s="22" t="s">
         <v>3</v>
       </c>
+      <c r="G270" s="22" t="s">
+        <v>1116</v>
+      </c>
       <c r="H270" s="18" t="str">
         <f t="shared" si="12"/>
         <v>public string fone_2_simp  { get; set; }</v>
@@ -20903,7 +20932,7 @@
       </c>
       <c r="J270" s="18" t="str">
         <f t="shared" si="14"/>
-        <v>|if(!string.IsNullOrWhiteSpace(msg.numeroTelefone2))| .fone_2_simp = msg.numeroTelefone2;</v>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.numeroTelefone2))| registroPessoaSimplificada.fone_2_simp = msg.numeroTelefone2;</v>
       </c>
     </row>
     <row r="271" spans="1:10" x14ac:dyDescent="0.25">
@@ -20923,6 +20952,9 @@
       <c r="F271" s="22" t="s">
         <v>3</v>
       </c>
+      <c r="G271" s="22" t="s">
+        <v>1116</v>
+      </c>
       <c r="H271" s="18" t="str">
         <f t="shared" si="12"/>
         <v>public string ram_fone_1_simp  { get; set; }</v>
@@ -20933,7 +20965,7 @@
       </c>
       <c r="J271" s="18" t="str">
         <f t="shared" si="14"/>
-        <v>|if(!string.IsNullOrWhiteSpace(msg.numeroRamal1))| .ram_fone_1_simp = msg.numeroRamal1;</v>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.numeroRamal1))| registroPessoaSimplificada.ram_fone_1_simp = msg.numeroRamal1;</v>
       </c>
     </row>
     <row r="272" spans="1:10" x14ac:dyDescent="0.25">
@@ -20953,6 +20985,9 @@
       <c r="F272" s="22" t="s">
         <v>3</v>
       </c>
+      <c r="G272" s="22" t="s">
+        <v>1116</v>
+      </c>
       <c r="H272" s="18" t="str">
         <f t="shared" si="12"/>
         <v>public string ram_fone_2_simp  { get; set; }</v>
@@ -20963,7 +20998,7 @@
       </c>
       <c r="J272" s="18" t="str">
         <f t="shared" si="14"/>
-        <v>|if(!string.IsNullOrWhiteSpace(msg.numeroRamal2))| .ram_fone_2_simp = msg.numeroRamal2;</v>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.numeroRamal2))| registroPessoaSimplificada.ram_fone_2_simp = msg.numeroRamal2;</v>
       </c>
     </row>
     <row r="273" spans="1:10" x14ac:dyDescent="0.25">
@@ -20983,6 +21018,9 @@
       <c r="F273" s="22" t="s">
         <v>3</v>
       </c>
+      <c r="G273" s="22" t="s">
+        <v>1116</v>
+      </c>
       <c r="H273" s="18" t="str">
         <f t="shared" si="12"/>
         <v>public string sit_fone_1_simp  { get; set; }</v>
@@ -20993,7 +21031,7 @@
       </c>
       <c r="J273" s="18" t="str">
         <f t="shared" si="14"/>
-        <v>|if(!string.IsNullOrWhiteSpace(msg.situacaoTelefone1))| .sit_fone_1_simp = msg.situacaoTelefone1;</v>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.situacaoTelefone1))| registroPessoaSimplificada.sit_fone_1_simp = msg.situacaoTelefone1;</v>
       </c>
     </row>
     <row r="274" spans="1:10" x14ac:dyDescent="0.25">
@@ -21013,6 +21051,9 @@
       <c r="F274" s="22" t="s">
         <v>3</v>
       </c>
+      <c r="G274" s="22" t="s">
+        <v>1116</v>
+      </c>
       <c r="H274" s="18" t="str">
         <f t="shared" si="12"/>
         <v>public string sit_fone_2_simp  { get; set; }</v>
@@ -21023,7 +21064,7 @@
       </c>
       <c r="J274" s="18" t="str">
         <f t="shared" si="14"/>
-        <v>|if(!string.IsNullOrWhiteSpace(msg.situacaoTelefone2))| .sit_fone_2_simp = msg.situacaoTelefone2;</v>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.situacaoTelefone2))| registroPessoaSimplificada.sit_fone_2_simp = msg.situacaoTelefone2;</v>
       </c>
     </row>
     <row r="275" spans="1:10" x14ac:dyDescent="0.25">
@@ -21043,6 +21084,9 @@
       <c r="F275" s="22" t="s">
         <v>1089</v>
       </c>
+      <c r="G275" s="22" t="s">
+        <v>1116</v>
+      </c>
       <c r="H275" s="18" t="str">
         <f t="shared" si="12"/>
         <v>public DateTime dat_nasc_simp  { get; set; }</v>
@@ -21053,7 +21097,7 @@
       </c>
       <c r="J275" s="18" t="str">
         <f t="shared" si="14"/>
-        <v>|if(msg.dataNascimento != DateTime.MinValue)| .dat_nasc_simp = msg.dataNascimento;</v>
+        <v>|if(msg.dataNascimento != DateTime.MinValue)| registroPessoaSimplificada.dat_nasc_simp = msg.dataNascimento;</v>
       </c>
     </row>
     <row r="276" spans="1:10" x14ac:dyDescent="0.25">
@@ -21073,6 +21117,9 @@
       <c r="F276" s="22" t="s">
         <v>3</v>
       </c>
+      <c r="G276" s="22" t="s">
+        <v>1116</v>
+      </c>
       <c r="H276" s="18" t="str">
         <f t="shared" si="12"/>
         <v>public string obs_simp  { get; set; }</v>
@@ -21083,7 +21130,7 @@
       </c>
       <c r="J276" s="18" t="str">
         <f t="shared" si="14"/>
-        <v>|if(!string.IsNullOrWhiteSpace(msg.observacao))| .obs_simp = msg.observacao;</v>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.observacao))| registroPessoaSimplificada.obs_simp = msg.observacao;</v>
       </c>
     </row>
     <row r="277" spans="1:10" x14ac:dyDescent="0.25">
@@ -21103,6 +21150,9 @@
       <c r="F277" s="22" t="s">
         <v>3</v>
       </c>
+      <c r="G277" s="22" t="s">
+        <v>1116</v>
+      </c>
       <c r="H277" s="18" t="str">
         <f t="shared" si="12"/>
         <v>public string tip_simp  { get; set; }</v>
@@ -21113,7 +21163,7 @@
       </c>
       <c r="J277" s="18" t="str">
         <f t="shared" si="14"/>
-        <v>|if(!string.IsNullOrWhiteSpace(msg.tipoReferencia))| .tip_simp = msg.tipoReferencia;</v>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.tipoReferencia))| registroPessoaSimplificada.tip_simp = msg.tipoReferencia;</v>
       </c>
     </row>
     <row r="278" spans="1:10" x14ac:dyDescent="0.25">
@@ -21133,6 +21183,9 @@
       <c r="F278" s="22" t="s">
         <v>1089</v>
       </c>
+      <c r="G278" s="22" t="s">
+        <v>1116</v>
+      </c>
       <c r="H278" s="18" t="str">
         <f t="shared" si="12"/>
         <v>public DateTime dat_cad  { get; set; }</v>
@@ -21143,7 +21196,7 @@
       </c>
       <c r="J278" s="18" t="str">
         <f t="shared" si="14"/>
-        <v>|if(msg.dataCadastramento != DateTime.MinValue)| .dat_cad = msg.dataCadastramento;</v>
+        <v>|if(msg.dataCadastramento != DateTime.MinValue)| registroPessoaSimplificada.dat_cad = msg.dataCadastramento;</v>
       </c>
     </row>
     <row r="279" spans="1:10" x14ac:dyDescent="0.25">
@@ -21163,6 +21216,9 @@
       <c r="F279" s="22" t="s">
         <v>3</v>
       </c>
+      <c r="G279" s="22" t="s">
+        <v>1116</v>
+      </c>
       <c r="H279" s="18" t="str">
         <f t="shared" si="12"/>
         <v>public string usu_atu  { get; set; }</v>
@@ -21173,7 +21229,7 @@
       </c>
       <c r="J279" s="18" t="str">
         <f t="shared" si="14"/>
-        <v>|if(!string.IsNullOrWhiteSpace(msg.usuarioUltimaAtualizacao))| .usu_atu = msg.usuarioUltimaAtualizacao;</v>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.usuarioUltimaAtualizacao))| registroPessoaSimplificada.usu_atu = msg.usuarioUltimaAtualizacao;</v>
       </c>
     </row>
     <row r="280" spans="1:10" x14ac:dyDescent="0.25">
@@ -21193,6 +21249,9 @@
       <c r="F280" s="22" t="s">
         <v>1089</v>
       </c>
+      <c r="G280" s="22" t="s">
+        <v>1116</v>
+      </c>
       <c r="H280" s="18" t="str">
         <f t="shared" si="12"/>
         <v>public DateTime dat_atu  { get; set; }</v>
@@ -21203,7 +21262,7 @@
       </c>
       <c r="J280" s="18" t="str">
         <f t="shared" si="14"/>
-        <v>|if(msg.dataAtualizacao != DateTime.MinValue)| .dat_atu = msg.dataAtualizacao;</v>
+        <v>|if(msg.dataAtualizacao != DateTime.MinValue)| registroPessoaSimplificada.dat_atu = msg.dataAtualizacao;</v>
       </c>
     </row>
     <row r="281" spans="1:10" x14ac:dyDescent="0.25">
@@ -21223,6 +21282,9 @@
       <c r="F281" s="22" t="s">
         <v>993</v>
       </c>
+      <c r="G281" s="22" t="s">
+        <v>1116</v>
+      </c>
       <c r="H281" s="18" t="str">
         <f t="shared" si="12"/>
         <v>public int cod_mun_simp  { get; set; }</v>
@@ -21233,7 +21295,7 @@
       </c>
       <c r="J281" s="18" t="str">
         <f t="shared" si="14"/>
-        <v>|if(msg.codigoMunicipio &gt; 0)| .cod_mun_simp = msg.codigoMunicipio;</v>
+        <v>|if(msg.codigoMunicipio &gt; 0)| registroPessoaSimplificada.cod_mun_simp = msg.codigoMunicipio;</v>
       </c>
     </row>
     <row r="282" spans="1:10" x14ac:dyDescent="0.25">
@@ -21253,6 +21315,9 @@
       <c r="F282" s="22" t="s">
         <v>3</v>
       </c>
+      <c r="G282" s="22" t="s">
+        <v>1116</v>
+      </c>
       <c r="H282" s="18" t="str">
         <f t="shared" si="12"/>
         <v>public string des_mun_simp  { get; set; }</v>
@@ -21263,7 +21328,7 @@
       </c>
       <c r="J282" s="18" t="str">
         <f t="shared" si="14"/>
-        <v>|if(!string.IsNullOrWhiteSpace(msg.descricaoMunicipio))| .des_mun_simp = msg.descricaoMunicipio;</v>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.descricaoMunicipio))| registroPessoaSimplificada.des_mun_simp = msg.descricaoMunicipio;</v>
       </c>
     </row>
     <row r="283" spans="1:10" x14ac:dyDescent="0.25">
@@ -21283,6 +21348,9 @@
       <c r="F283" s="22" t="s">
         <v>3</v>
       </c>
+      <c r="G283" s="22" t="s">
+        <v>1116</v>
+      </c>
       <c r="H283" s="18" t="str">
         <f t="shared" si="12"/>
         <v>public string tip_log_simp  { get; set; }</v>
@@ -21293,7 +21361,7 @@
       </c>
       <c r="J283" s="18" t="str">
         <f t="shared" si="14"/>
-        <v>|if(!string.IsNullOrWhiteSpace(msg.tipoLogradouro))| .tip_log_simp = msg.tipoLogradouro;</v>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.tipoLogradouro))| registroPessoaSimplificada.tip_log_simp = msg.tipoLogradouro;</v>
       </c>
     </row>
     <row r="284" spans="1:10" x14ac:dyDescent="0.25">
@@ -21313,6 +21381,9 @@
       <c r="F284" s="22" t="s">
         <v>3</v>
       </c>
+      <c r="G284" s="22" t="s">
+        <v>1116</v>
+      </c>
       <c r="H284" s="18" t="str">
         <f t="shared" si="12"/>
         <v>public string des_log_simp  { get; set; }</v>
@@ -21323,7 +21394,7 @@
       </c>
       <c r="J284" s="18" t="str">
         <f t="shared" si="14"/>
-        <v>|if(!string.IsNullOrWhiteSpace(msg.descricicaoLogradouro))| .des_log_simp = msg.descricicaoLogradouro;</v>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.descricicaoLogradouro))| registroPessoaSimplificada.des_log_simp = msg.descricicaoLogradouro;</v>
       </c>
     </row>
     <row r="285" spans="1:10" x14ac:dyDescent="0.25">
@@ -21343,6 +21414,9 @@
       <c r="F285" s="22" t="s">
         <v>3</v>
       </c>
+      <c r="G285" s="22" t="s">
+        <v>1116</v>
+      </c>
       <c r="H285" s="18" t="str">
         <f t="shared" si="12"/>
         <v>public string num_simp  { get; set; }</v>
@@ -21353,7 +21427,7 @@
       </c>
       <c r="J285" s="18" t="str">
         <f t="shared" si="14"/>
-        <v>|if(!string.IsNullOrWhiteSpace(msg.numeroEndereco))| .num_simp = msg.numeroEndereco;</v>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.numeroEndereco))| registroPessoaSimplificada.num_simp = msg.numeroEndereco;</v>
       </c>
     </row>
     <row r="286" spans="1:10" x14ac:dyDescent="0.25">
@@ -21373,6 +21447,9 @@
       <c r="F286" s="22" t="s">
         <v>3</v>
       </c>
+      <c r="G286" s="22" t="s">
+        <v>1116</v>
+      </c>
       <c r="H286" s="18" t="str">
         <f t="shared" si="12"/>
         <v>public string cpl_end_simp  { get; set; }</v>
@@ -21383,7 +21460,7 @@
       </c>
       <c r="J286" s="18" t="str">
         <f t="shared" si="14"/>
-        <v>|if(!string.IsNullOrWhiteSpace(msg.complementoLogradouro))| .cpl_end_simp = msg.complementoLogradouro;</v>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.complementoLogradouro))| registroPessoaSimplificada.cpl_end_simp = msg.complementoLogradouro;</v>
       </c>
     </row>
     <row r="287" spans="1:10" x14ac:dyDescent="0.25">
@@ -21403,6 +21480,9 @@
       <c r="F287" s="22" t="s">
         <v>3</v>
       </c>
+      <c r="G287" s="22" t="s">
+        <v>1116</v>
+      </c>
       <c r="H287" s="18" t="str">
         <f t="shared" si="12"/>
         <v>public string bai_end_simp  { get; set; }</v>
@@ -21413,7 +21493,7 @@
       </c>
       <c r="J287" s="18" t="str">
         <f t="shared" si="14"/>
-        <v>|if(!string.IsNullOrWhiteSpace(msg.nomeBairro))| .bai_end_simp = msg.nomeBairro;</v>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.nomeBairro))| registroPessoaSimplificada.bai_end_simp = msg.nomeBairro;</v>
       </c>
     </row>
     <row r="288" spans="1:10" x14ac:dyDescent="0.25">
@@ -21433,6 +21513,9 @@
       <c r="F288" s="22" t="s">
         <v>3</v>
       </c>
+      <c r="G288" s="22" t="s">
+        <v>1116</v>
+      </c>
       <c r="H288" s="18" t="str">
         <f t="shared" si="12"/>
         <v>public string tip_end_simp  { get; set; }</v>
@@ -21443,7 +21526,7 @@
       </c>
       <c r="J288" s="18" t="str">
         <f t="shared" si="14"/>
-        <v>|if(!string.IsNullOrWhiteSpace(msg.tipoEndereco))| .tip_end_simp = msg.tipoEndereco;</v>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.tipoEndereco))| registroPessoaSimplificada.tip_end_simp = msg.tipoEndereco;</v>
       </c>
     </row>
     <row r="289" spans="1:10" x14ac:dyDescent="0.25">
@@ -21463,6 +21546,9 @@
       <c r="F289" s="22" t="s">
         <v>3</v>
       </c>
+      <c r="G289" s="22" t="s">
+        <v>1116</v>
+      </c>
       <c r="H289" s="18" t="str">
         <f t="shared" si="12"/>
         <v>public string uf_end_simp  { get; set; }</v>
@@ -21473,7 +21559,7 @@
       </c>
       <c r="J289" s="18" t="str">
         <f t="shared" si="14"/>
-        <v>|if(!string.IsNullOrWhiteSpace(msg.uf))| .uf_end_simp = msg.uf;</v>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.uf))| registroPessoaSimplificada.uf_end_simp = msg.uf;</v>
       </c>
     </row>
     <row r="290" spans="1:10" x14ac:dyDescent="0.25">
@@ -21493,6 +21579,9 @@
       <c r="F290" s="22" t="s">
         <v>3</v>
       </c>
+      <c r="G290" s="22" t="s">
+        <v>1116</v>
+      </c>
       <c r="H290" s="18" t="str">
         <f t="shared" si="12"/>
         <v>public string pais_simp  { get; set; }</v>
@@ -21503,7 +21592,7 @@
       </c>
       <c r="J290" s="18" t="str">
         <f t="shared" si="14"/>
-        <v>|if(!string.IsNullOrWhiteSpace(msg.pais))| .pais_simp = msg.pais;</v>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.pais))| registroPessoaSimplificada.pais_simp = msg.pais;</v>
       </c>
     </row>
     <row r="291" spans="1:10" x14ac:dyDescent="0.25">
@@ -21523,6 +21612,9 @@
       <c r="F291" s="22" t="s">
         <v>3</v>
       </c>
+      <c r="G291" s="22" t="s">
+        <v>1116</v>
+      </c>
       <c r="H291" s="18" t="str">
         <f t="shared" si="12"/>
         <v>public string cep_simp  { get; set; }</v>
@@ -21533,7 +21625,7 @@
       </c>
       <c r="J291" s="18" t="str">
         <f t="shared" si="14"/>
-        <v>|if(!string.IsNullOrWhiteSpace(msg.numeroCep))| .cep_simp = msg.numeroCep;</v>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.numeroCep))| registroPessoaSimplificada.cep_simp = msg.numeroCep;</v>
       </c>
     </row>
     <row r="292" spans="1:10" x14ac:dyDescent="0.25">
@@ -21553,6 +21645,9 @@
       <c r="F292" s="22" t="s">
         <v>3</v>
       </c>
+      <c r="G292" s="22" t="s">
+        <v>1116</v>
+      </c>
       <c r="H292" s="18" t="str">
         <f t="shared" ref="H292:H355" si="15">CONCATENATE("public ",F292," ",B292,"  { get; set; }")</f>
         <v>public string est_civ_simp  { get; set; }</v>
@@ -21563,7 +21658,7 @@
       </c>
       <c r="J292" s="18" t="str">
         <f t="shared" si="14"/>
-        <v>|if(!string.IsNullOrWhiteSpace(msg.estadoCivil))| .est_civ_simp = msg.estadoCivil;</v>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.estadoCivil))| registroPessoaSimplificada.est_civ_simp = msg.estadoCivil;</v>
       </c>
     </row>
     <row r="293" spans="1:10" x14ac:dyDescent="0.25">
@@ -21583,6 +21678,9 @@
       <c r="F293" s="22" t="s">
         <v>3</v>
       </c>
+      <c r="G293" s="22" t="s">
+        <v>1116</v>
+      </c>
       <c r="H293" s="18" t="str">
         <f t="shared" si="15"/>
         <v>public string reg_com_simp  { get; set; }</v>
@@ -21593,7 +21691,7 @@
       </c>
       <c r="J293" s="18" t="str">
         <f t="shared" si="14"/>
-        <v>|if(!string.IsNullOrWhiteSpace(msg.regimeComunhao))| .reg_com_simp = msg.regimeComunhao;</v>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.regimeComunhao))| registroPessoaSimplificada.reg_com_simp = msg.regimeComunhao;</v>
       </c>
     </row>
     <row r="294" spans="1:10" x14ac:dyDescent="0.25">
@@ -21613,6 +21711,9 @@
       <c r="F294" s="22" t="s">
         <v>3</v>
       </c>
+      <c r="G294" s="22" t="s">
+        <v>1116</v>
+      </c>
       <c r="H294" s="18" t="str">
         <f t="shared" si="15"/>
         <v>public string nom_conj_simp  { get; set; }</v>
@@ -21623,7 +21724,7 @@
       </c>
       <c r="J294" s="18" t="str">
         <f t="shared" si="14"/>
-        <v>|if(!string.IsNullOrWhiteSpace(msg.nomeConjugue))| .nom_conj_simp = msg.nomeConjugue;</v>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.nomeConjugue))| registroPessoaSimplificada.nom_conj_simp = msg.nomeConjugue;</v>
       </c>
     </row>
     <row r="295" spans="1:10" x14ac:dyDescent="0.25">
@@ -21643,6 +21744,9 @@
       <c r="F295" s="22" t="s">
         <v>3</v>
       </c>
+      <c r="G295" s="22" t="s">
+        <v>1116</v>
+      </c>
       <c r="H295" s="18" t="str">
         <f t="shared" si="15"/>
         <v>public string idc_ava_simp  { get; set; }</v>
@@ -21653,7 +21757,7 @@
       </c>
       <c r="J295" s="18" t="str">
         <f t="shared" si="14"/>
-        <v>|if(!string.IsNullOrWhiteSpace(msg.indicadorAvalista))| .idc_ava_simp = msg.indicadorAvalista;</v>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.indicadorAvalista))| registroPessoaSimplificada.idc_ava_simp = msg.indicadorAvalista;</v>
       </c>
     </row>
     <row r="296" spans="1:10" x14ac:dyDescent="0.25">
@@ -21673,6 +21777,9 @@
       <c r="F296" s="22" t="s">
         <v>3</v>
       </c>
+      <c r="G296" s="22" t="s">
+        <v>1116</v>
+      </c>
       <c r="H296" s="18" t="str">
         <f t="shared" si="15"/>
         <v>public string cpf_cnpj_simp  { get; set; }</v>
@@ -21683,7 +21790,7 @@
       </c>
       <c r="J296" s="18" t="str">
         <f t="shared" si="14"/>
-        <v>|if(!string.IsNullOrWhiteSpace(msg.CpfCnpjSimplificado))| .cpf_cnpj_simp = msg.CpfCnpjSimplificado;</v>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.CpfCnpjSimplificado))| registroPessoaSimplificada.cpf_cnpj_simp = msg.CpfCnpjSimplificado;</v>
       </c>
     </row>
     <row r="297" spans="1:10" x14ac:dyDescent="0.25">
@@ -21703,6 +21810,9 @@
       <c r="F297" s="22" t="s">
         <v>3</v>
       </c>
+      <c r="G297" s="22" t="s">
+        <v>1116</v>
+      </c>
       <c r="H297" s="18" t="str">
         <f t="shared" si="15"/>
         <v>public string tip_pes_simp  { get; set; }</v>
@@ -21713,7 +21823,7 @@
       </c>
       <c r="J297" s="18" t="str">
         <f t="shared" si="14"/>
-        <v>|if(!string.IsNullOrWhiteSpace(msg.tipoPessoa))| .tip_pes_simp = msg.tipoPessoa;</v>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.tipoPessoa))| registroPessoaSimplificada.tip_pes_simp = msg.tipoPessoa;</v>
       </c>
     </row>
     <row r="298" spans="1:10" x14ac:dyDescent="0.25">
@@ -21733,6 +21843,9 @@
       <c r="F298" s="22" t="s">
         <v>3</v>
       </c>
+      <c r="G298" s="22" t="s">
+        <v>1116</v>
+      </c>
       <c r="H298" s="18" t="str">
         <f t="shared" si="15"/>
         <v>public string idc_isen_cpf_cnpf_simp  { get; set; }</v>
@@ -21743,7 +21856,7 @@
       </c>
       <c r="J298" s="18" t="str">
         <f t="shared" si="14"/>
-        <v>|if(!string.IsNullOrWhiteSpace(msg.identificadorIsentoCpf))| .idc_isen_cpf_cnpf_simp = msg.identificadorIsentoCpf;</v>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.identificadorIsentoCpf))| registroPessoaSimplificada.idc_isen_cpf_cnpf_simp = msg.identificadorIsentoCpf;</v>
       </c>
     </row>
     <row r="299" spans="1:10" x14ac:dyDescent="0.25">
@@ -21763,6 +21876,9 @@
       <c r="F299" s="22" t="s">
         <v>3</v>
       </c>
+      <c r="G299" s="22" t="s">
+        <v>1116</v>
+      </c>
       <c r="H299" s="18" t="str">
         <f t="shared" si="15"/>
         <v>public string pescodsisorigem  { get; set; }</v>
@@ -21773,7 +21889,7 @@
       </c>
       <c r="J299" s="18" t="str">
         <f t="shared" si="14"/>
-        <v>|if(!string.IsNullOrWhiteSpace(msg.codigoSistemaOrigem))| .pescodsisorigem = msg.codigoSistemaOrigem;</v>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.codigoSistemaOrigem))| registroPessoaSimplificada.pescodsisorigem = msg.codigoSistemaOrigem;</v>
       </c>
     </row>
     <row r="300" spans="1:10" x14ac:dyDescent="0.25">
@@ -21793,6 +21909,9 @@
       <c r="F300" s="22" t="s">
         <v>3</v>
       </c>
+      <c r="G300" s="22" t="s">
+        <v>1116</v>
+      </c>
       <c r="H300" s="18" t="str">
         <f t="shared" si="15"/>
         <v>public string pescpfconj  { get; set; }</v>
@@ -21803,7 +21922,7 @@
       </c>
       <c r="J300" s="18" t="str">
         <f t="shared" si="14"/>
-        <v>|if(!string.IsNullOrWhiteSpace(msg.CpfConjugue))| .pescpfconj = msg.CpfConjugue;</v>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.CpfConjugue))| registroPessoaSimplificada.pescpfconj = msg.CpfConjugue;</v>
       </c>
     </row>
     <row r="301" spans="1:10" x14ac:dyDescent="0.25">
@@ -21823,6 +21942,9 @@
       <c r="F301" s="22" t="s">
         <v>3</v>
       </c>
+      <c r="G301" s="22" t="s">
+        <v>1116</v>
+      </c>
       <c r="H301" s="18" t="str">
         <f t="shared" si="15"/>
         <v>public string idc_fatca  { get; set; }</v>
@@ -21833,7 +21955,7 @@
       </c>
       <c r="J301" s="18" t="str">
         <f t="shared" si="14"/>
-        <v>|if(!string.IsNullOrWhiteSpace(msg.indicadorClienteFatca))| .idc_fatca = msg.indicadorClienteFatca;</v>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.indicadorClienteFatca))| registroPessoaSimplificada.idc_fatca = msg.indicadorClienteFatca;</v>
       </c>
     </row>
     <row r="302" spans="1:10" x14ac:dyDescent="0.25">
@@ -21853,6 +21975,9 @@
       <c r="F302" s="22" t="s">
         <v>3</v>
       </c>
+      <c r="G302" s="22" t="s">
+        <v>1116</v>
+      </c>
       <c r="H302" s="18" t="str">
         <f t="shared" si="15"/>
         <v>public string rg_simp  { get; set; }</v>
@@ -21863,7 +21988,7 @@
       </c>
       <c r="J302" s="18" t="str">
         <f t="shared" si="14"/>
-        <v>|if(!string.IsNullOrWhiteSpace(msg.numeroRg))| .rg_simp = msg.numeroRg;</v>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.numeroRg))| registroPessoaSimplificada.rg_simp = msg.numeroRg;</v>
       </c>
     </row>
     <row r="303" spans="1:10" x14ac:dyDescent="0.25">
@@ -21883,6 +22008,9 @@
       <c r="F303" s="22" t="s">
         <v>3</v>
       </c>
+      <c r="G303" s="22" t="s">
+        <v>1116</v>
+      </c>
       <c r="H303" s="18" t="str">
         <f t="shared" si="15"/>
         <v>public string nif_simp  { get; set; }</v>
@@ -21893,7 +22021,7 @@
       </c>
       <c r="J303" s="18" t="str">
         <f t="shared" si="14"/>
-        <v>|if(!string.IsNullOrWhiteSpace(msg.numeroIdentificadorFiscal))| .nif_simp = msg.numeroIdentificadorFiscal;</v>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.numeroIdentificadorFiscal))| registroPessoaSimplificada.nif_simp = msg.numeroIdentificadorFiscal;</v>
       </c>
     </row>
     <row r="304" spans="1:10" x14ac:dyDescent="0.25">
@@ -21913,6 +22041,9 @@
       <c r="F304" s="22" t="s">
         <v>993</v>
       </c>
+      <c r="G304" s="22" t="s">
+        <v>1116</v>
+      </c>
       <c r="H304" s="18" t="str">
         <f t="shared" si="15"/>
         <v>public int nac1_simp  { get; set; }</v>
@@ -21923,7 +22054,7 @@
       </c>
       <c r="J304" s="18" t="str">
         <f t="shared" si="14"/>
-        <v>|if(msg.codigoNacionalidade1 &gt; 0)| .nac1_simp = msg.codigoNacionalidade1;</v>
+        <v>|if(msg.codigoNacionalidade1 &gt; 0)| registroPessoaSimplificada.nac1_simp = msg.codigoNacionalidade1;</v>
       </c>
     </row>
     <row r="305" spans="1:10" x14ac:dyDescent="0.25">
@@ -21943,6 +22074,9 @@
       <c r="F305" s="22" t="s">
         <v>993</v>
       </c>
+      <c r="G305" s="22" t="s">
+        <v>1116</v>
+      </c>
       <c r="H305" s="18" t="str">
         <f t="shared" si="15"/>
         <v>public int nac2_simp  { get; set; }</v>
@@ -21953,7 +22087,7 @@
       </c>
       <c r="J305" s="18" t="str">
         <f t="shared" si="14"/>
-        <v>|if(msg.codigoNacionalidade2 &gt; 0)| .nac2_simp = msg.codigoNacionalidade2;</v>
+        <v>|if(msg.codigoNacionalidade2 &gt; 0)| registroPessoaSimplificada.nac2_simp = msg.codigoNacionalidade2;</v>
       </c>
     </row>
     <row r="306" spans="1:10" x14ac:dyDescent="0.25">
@@ -21973,6 +22107,9 @@
       <c r="F306" s="22" t="s">
         <v>993</v>
       </c>
+      <c r="G306" s="22" t="s">
+        <v>1116</v>
+      </c>
       <c r="H306" s="18" t="str">
         <f t="shared" si="15"/>
         <v>public int nac3_simp  { get; set; }</v>
@@ -21983,7 +22120,7 @@
       </c>
       <c r="J306" s="18" t="str">
         <f t="shared" si="14"/>
-        <v>|if(msg.codigoNacionalidade3 &gt; 0)| .nac3_simp = msg.codigoNacionalidade3;</v>
+        <v>|if(msg.codigoNacionalidade3 &gt; 0)| registroPessoaSimplificada.nac3_simp = msg.codigoNacionalidade3;</v>
       </c>
     </row>
     <row r="307" spans="1:10" x14ac:dyDescent="0.25">
@@ -22003,6 +22140,9 @@
       <c r="F307" s="22" t="s">
         <v>993</v>
       </c>
+      <c r="G307" s="22" t="s">
+        <v>1116</v>
+      </c>
       <c r="H307" s="18" t="str">
         <f t="shared" si="15"/>
         <v>public int nac4_simp  { get; set; }</v>
@@ -22013,7 +22153,7 @@
       </c>
       <c r="J307" s="18" t="str">
         <f t="shared" si="14"/>
-        <v>|if(msg.codigoNacionalidade4 &gt; 0)| .nac4_simp = msg.codigoNacionalidade4;</v>
+        <v>|if(msg.codigoNacionalidade4 &gt; 0)| registroPessoaSimplificada.nac4_simp = msg.codigoNacionalidade4;</v>
       </c>
     </row>
     <row r="308" spans="1:10" x14ac:dyDescent="0.25">
@@ -22033,6 +22173,9 @@
       <c r="F308" s="22" t="s">
         <v>993</v>
       </c>
+      <c r="G308" s="22" t="s">
+        <v>1116</v>
+      </c>
       <c r="H308" s="18" t="str">
         <f t="shared" si="15"/>
         <v>public int dom_fis1_simp  { get; set; }</v>
@@ -22043,7 +22186,7 @@
       </c>
       <c r="J308" s="18" t="str">
         <f t="shared" si="14"/>
-        <v>|if(msg.codigoDomicilioFiscal1 &gt; 0)| .dom_fis1_simp = msg.codigoDomicilioFiscal1;</v>
+        <v>|if(msg.codigoDomicilioFiscal1 &gt; 0)| registroPessoaSimplificada.dom_fis1_simp = msg.codigoDomicilioFiscal1;</v>
       </c>
     </row>
     <row r="309" spans="1:10" x14ac:dyDescent="0.25">
@@ -22063,6 +22206,9 @@
       <c r="F309" s="22" t="s">
         <v>993</v>
       </c>
+      <c r="G309" s="22" t="s">
+        <v>1116</v>
+      </c>
       <c r="H309" s="18" t="str">
         <f t="shared" si="15"/>
         <v>public int dom_fis2_simp  { get; set; }</v>
@@ -22073,7 +22219,7 @@
       </c>
       <c r="J309" s="18" t="str">
         <f t="shared" si="14"/>
-        <v>|if(msg.codigoDomicilioFiscal2 &gt; 0)| .dom_fis2_simp = msg.codigoDomicilioFiscal2;</v>
+        <v>|if(msg.codigoDomicilioFiscal2 &gt; 0)| registroPessoaSimplificada.dom_fis2_simp = msg.codigoDomicilioFiscal2;</v>
       </c>
     </row>
     <row r="310" spans="1:10" x14ac:dyDescent="0.25">
@@ -22093,6 +22239,9 @@
       <c r="F310" s="22" t="s">
         <v>993</v>
       </c>
+      <c r="G310" s="22" t="s">
+        <v>1116</v>
+      </c>
       <c r="H310" s="18" t="str">
         <f t="shared" si="15"/>
         <v>public int dom_fis3_simp  { get; set; }</v>
@@ -22103,7 +22252,7 @@
       </c>
       <c r="J310" s="18" t="str">
         <f t="shared" si="14"/>
-        <v>|if(msg.codigoDomicilioFiscal3 &gt; 0)| .dom_fis3_simp = msg.codigoDomicilioFiscal3;</v>
+        <v>|if(msg.codigoDomicilioFiscal3 &gt; 0)| registroPessoaSimplificada.dom_fis3_simp = msg.codigoDomicilioFiscal3;</v>
       </c>
     </row>
     <row r="311" spans="1:10" x14ac:dyDescent="0.25">
@@ -22123,6 +22272,9 @@
       <c r="F311" s="22" t="s">
         <v>993</v>
       </c>
+      <c r="G311" s="22" t="s">
+        <v>1116</v>
+      </c>
       <c r="H311" s="18" t="str">
         <f t="shared" si="15"/>
         <v>public int dom_fis4_simp  { get; set; }</v>
@@ -22133,7 +22285,7 @@
       </c>
       <c r="J311" s="18" t="str">
         <f t="shared" si="14"/>
-        <v>|if(msg.codigoDomicilioFiscal4 &gt; 0)| .dom_fis4_simp = msg.codigoDomicilioFiscal4;</v>
+        <v>|if(msg.codigoDomicilioFiscal4 &gt; 0)| registroPessoaSimplificada.dom_fis4_simp = msg.codigoDomicilioFiscal4;</v>
       </c>
     </row>
     <row r="312" spans="1:10" x14ac:dyDescent="0.25">
@@ -22153,6 +22305,9 @@
       <c r="F312" s="22" t="s">
         <v>3</v>
       </c>
+      <c r="G312" s="22" t="s">
+        <v>1116</v>
+      </c>
       <c r="H312" s="18" t="str">
         <f t="shared" si="15"/>
         <v>public string ddd_cel_simp  { get; set; }</v>
@@ -22163,7 +22318,7 @@
       </c>
       <c r="J312" s="18" t="str">
         <f t="shared" si="14"/>
-        <v>|if(!string.IsNullOrWhiteSpace(msg.codigoDddCelular))| .ddd_cel_simp = msg.codigoDddCelular;</v>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.codigoDddCelular))| registroPessoaSimplificada.ddd_cel_simp = msg.codigoDddCelular;</v>
       </c>
     </row>
     <row r="313" spans="1:10" x14ac:dyDescent="0.25">
@@ -22183,6 +22338,9 @@
       <c r="F313" s="22" t="s">
         <v>3</v>
       </c>
+      <c r="G313" s="22" t="s">
+        <v>1116</v>
+      </c>
       <c r="H313" s="18" t="str">
         <f t="shared" si="15"/>
         <v>public string fone_cel_simp  { get; set; }</v>
@@ -22193,7 +22351,7 @@
       </c>
       <c r="J313" s="18" t="str">
         <f t="shared" si="14"/>
-        <v>|if(!string.IsNullOrWhiteSpace(msg.numeroCelular))| .fone_cel_simp = msg.numeroCelular;</v>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.numeroCelular))| registroPessoaSimplificada.fone_cel_simp = msg.numeroCelular;</v>
       </c>
     </row>
     <row r="314" spans="1:10" x14ac:dyDescent="0.25">
@@ -22213,6 +22371,9 @@
       <c r="F314" s="22" t="s">
         <v>3</v>
       </c>
+      <c r="G314" s="22" t="s">
+        <v>1116</v>
+      </c>
       <c r="H314" s="18" t="str">
         <f t="shared" si="15"/>
         <v>public string email  { get; set; }</v>
@@ -22223,7 +22384,7 @@
       </c>
       <c r="J314" s="18" t="str">
         <f t="shared" si="14"/>
-        <v>|if(!string.IsNullOrWhiteSpace(msg.email))| .email = msg.email;</v>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.email))| registroPessoaSimplificada.email = msg.email;</v>
       </c>
     </row>
     <row r="315" spans="1:10" x14ac:dyDescent="0.25">
@@ -22243,6 +22404,9 @@
       <c r="F315" s="22" t="s">
         <v>3</v>
       </c>
+      <c r="G315" s="22" t="s">
+        <v>1116</v>
+      </c>
       <c r="H315" s="18" t="str">
         <f t="shared" si="15"/>
         <v>public string idc_cli_est  { get; set; }</v>
@@ -22253,7 +22417,7 @@
       </c>
       <c r="J315" s="18" t="str">
         <f t="shared" si="14"/>
-        <v>|if(!string.IsNullOrWhiteSpace(msg.indicadorClienteEstrangeiro))| .idc_cli_est = msg.indicadorClienteEstrangeiro;</v>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.indicadorClienteEstrangeiro))| registroPessoaSimplificada.idc_cli_est = msg.indicadorClienteEstrangeiro;</v>
       </c>
     </row>
     <row r="316" spans="1:10" x14ac:dyDescent="0.25">
@@ -22273,6 +22437,9 @@
       <c r="F316" s="22" t="s">
         <v>3</v>
       </c>
+      <c r="G316" s="22" t="s">
+        <v>1116</v>
+      </c>
       <c r="H316" s="18" t="str">
         <f t="shared" si="15"/>
         <v>public string tip_doc_est  { get; set; }</v>
@@ -22283,7 +22450,7 @@
       </c>
       <c r="J316" s="18" t="str">
         <f t="shared" si="14"/>
-        <v>|if(!string.IsNullOrWhiteSpace(msg.tipoDocumentoEstrangeiro))| .tip_doc_est = msg.tipoDocumentoEstrangeiro;</v>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.tipoDocumentoEstrangeiro))| registroPessoaSimplificada.tip_doc_est = msg.tipoDocumentoEstrangeiro;</v>
       </c>
     </row>
     <row r="317" spans="1:10" x14ac:dyDescent="0.25">
@@ -22303,6 +22470,9 @@
       <c r="F317" s="22" t="s">
         <v>3</v>
       </c>
+      <c r="G317" s="22" t="s">
+        <v>1116</v>
+      </c>
       <c r="H317" s="18" t="str">
         <f t="shared" si="15"/>
         <v>public string num_doc_est  { get; set; }</v>
@@ -22313,7 +22483,7 @@
       </c>
       <c r="J317" s="18" t="str">
         <f t="shared" si="14"/>
-        <v>|if(!string.IsNullOrWhiteSpace(msg.numeroDocumentoEstrangeiro))| .num_doc_est = msg.numeroDocumentoEstrangeiro;</v>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.numeroDocumentoEstrangeiro))| registroPessoaSimplificada.num_doc_est = msg.numeroDocumentoEstrangeiro;</v>
       </c>
     </row>
     <row r="318" spans="1:10" x14ac:dyDescent="0.25">
@@ -22333,6 +22503,9 @@
       <c r="F318" s="21" t="s">
         <v>3</v>
       </c>
+      <c r="G318" s="22" t="s">
+        <v>1116</v>
+      </c>
       <c r="H318" s="18" t="str">
         <f t="shared" si="15"/>
         <v>public string nom_social_simp  { get; set; }</v>
@@ -22343,7 +22516,7 @@
       </c>
       <c r="J318" s="18" t="str">
         <f t="shared" si="14"/>
-        <v>|if(!string.IsNullOrWhiteSpace(msg.nomeSocial))| .nom_social_simp = msg.nomeSocial;</v>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.nomeSocial))| registroPessoaSimplificada.nom_social_simp = msg.nomeSocial;</v>
       </c>
     </row>
     <row r="319" spans="1:10" x14ac:dyDescent="0.25">
@@ -22363,6 +22536,9 @@
       <c r="F319" s="21" t="s">
         <v>3</v>
       </c>
+      <c r="G319" s="22" t="s">
+        <v>1116</v>
+      </c>
       <c r="H319" s="18" t="str">
         <f t="shared" si="15"/>
         <v>public string pld_pes  { get; set; }</v>
@@ -22373,7 +22549,7 @@
       </c>
       <c r="J319" s="18" t="str">
         <f t="shared" si="14"/>
-        <v>|if(!string.IsNullOrWhiteSpace(msg.nivelRiscoPld))| .pld_pes = msg.nivelRiscoPld;</v>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.nivelRiscoPld))| registroPessoaSimplificada.pld_pes = msg.nivelRiscoPld;</v>
       </c>
     </row>
     <row r="320" spans="1:10" x14ac:dyDescent="0.25">
@@ -22393,6 +22569,9 @@
       <c r="F320" s="21" t="s">
         <v>3</v>
       </c>
+      <c r="G320" s="22" t="s">
+        <v>1116</v>
+      </c>
       <c r="H320" s="18" t="str">
         <f t="shared" si="15"/>
         <v>public string obs_pld  { get; set; }</v>
@@ -22403,7 +22582,7 @@
       </c>
       <c r="J320" s="18" t="str">
         <f t="shared" si="14"/>
-        <v>|if(!string.IsNullOrWhiteSpace(msg.observacaoPld))| .obs_pld = msg.observacaoPld;</v>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.observacaoPld))| registroPessoaSimplificada.obs_pld = msg.observacaoPld;</v>
       </c>
     </row>
     <row r="321" spans="1:10" x14ac:dyDescent="0.25">
@@ -22425,6 +22604,9 @@
       <c r="F321" s="13" t="s">
         <v>3</v>
       </c>
+      <c r="G321" s="22" t="s">
+        <v>1116</v>
+      </c>
       <c r="H321" s="18" t="str">
         <f t="shared" si="15"/>
         <v>public string cod_cbo  { get; set; }</v>
@@ -22435,7 +22617,7 @@
       </c>
       <c r="J321" s="18" t="str">
         <f t="shared" si="14"/>
-        <v>|if(!string.IsNullOrWhiteSpace(msg.CodigoAtividadeCbo))| .cod_cbo = msg.CodigoAtividadeCbo;</v>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.CodigoAtividadeCbo))| registroPessoaSimplificada.cod_cbo = msg.CodigoAtividadeCbo;</v>
       </c>
     </row>
     <row r="322" spans="1:10" x14ac:dyDescent="0.25">
@@ -22454,6 +22636,9 @@
       <c r="F322" s="19" t="s">
         <v>993</v>
       </c>
+      <c r="G322" s="22" t="s">
+        <v>1116</v>
+      </c>
       <c r="H322" s="18" t="str">
         <f t="shared" si="15"/>
         <v>public int COD_ATIVIDADE  { get; set; }</v>
@@ -22464,7 +22649,7 @@
       </c>
       <c r="J322" s="18" t="str">
         <f t="shared" si="14"/>
-        <v>|if(msg.CodigoAtividade &gt; 0)| .COD_ATIVIDADE = msg.CodigoAtividade;</v>
+        <v>|if(msg.CodigoAtividade &gt; 0)| registroPessoaSimplificada.COD_ATIVIDADE = msg.CodigoAtividade;</v>
       </c>
     </row>
     <row r="323" spans="1:10" x14ac:dyDescent="0.25">
@@ -22486,6 +22671,9 @@
       <c r="F323" s="22" t="s">
         <v>3</v>
       </c>
+      <c r="G323" s="22" t="s">
+        <v>1114</v>
+      </c>
       <c r="H323" s="18" t="str">
         <f t="shared" si="15"/>
         <v>public string cod_pessoa_jur  { get; set; }</v>
@@ -22496,7 +22684,7 @@
       </c>
       <c r="J323" s="18" t="str">
         <f t="shared" ref="J323:J363" si="17">CONCATENATE("|if(",I323,")","| ",G323,".",B323," = msg.",E323,";")</f>
-        <v>|if(!string.IsNullOrWhiteSpace(msg.codigoPessoaJuridica))| .cod_pessoa_jur = msg.codigoPessoaJuridica;</v>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.codigoPessoaJuridica))| registroVinculo.cod_pessoa_jur = msg.codigoPessoaJuridica;</v>
       </c>
     </row>
     <row r="324" spans="1:10" x14ac:dyDescent="0.25">
@@ -22518,6 +22706,9 @@
       <c r="F324" s="22" t="s">
         <v>3</v>
       </c>
+      <c r="G324" s="22" t="s">
+        <v>1114</v>
+      </c>
       <c r="H324" s="18" t="str">
         <f t="shared" si="15"/>
         <v>public string cod_fil_jur  { get; set; }</v>
@@ -22528,7 +22719,7 @@
       </c>
       <c r="J324" s="18" t="str">
         <f t="shared" si="17"/>
-        <v>|if(!string.IsNullOrWhiteSpace(msg.codigoFilialPessoaJuridica))| .cod_fil_jur = msg.codigoFilialPessoaJuridica;</v>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.codigoFilialPessoaJuridica))| registroVinculo.cod_fil_jur = msg.codigoFilialPessoaJuridica;</v>
       </c>
     </row>
     <row r="325" spans="1:10" x14ac:dyDescent="0.25">
@@ -22550,6 +22741,9 @@
       <c r="F325" s="22" t="s">
         <v>3</v>
       </c>
+      <c r="G325" s="22" t="s">
+        <v>1114</v>
+      </c>
       <c r="H325" s="18" t="str">
         <f t="shared" si="15"/>
         <v>public string cod_pessoa_fis  { get; set; }</v>
@@ -22560,7 +22754,7 @@
       </c>
       <c r="J325" s="18" t="str">
         <f t="shared" si="17"/>
-        <v>|if(!string.IsNullOrWhiteSpace(msg.codigoPessoaFisica))| .cod_pessoa_fis = msg.codigoPessoaFisica;</v>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.codigoPessoaFisica))| registroVinculo.cod_pessoa_fis = msg.codigoPessoaFisica;</v>
       </c>
     </row>
     <row r="326" spans="1:10" x14ac:dyDescent="0.25">
@@ -22582,6 +22776,9 @@
       <c r="F326" s="22" t="s">
         <v>3</v>
       </c>
+      <c r="G326" s="22" t="s">
+        <v>1114</v>
+      </c>
       <c r="H326" s="18" t="str">
         <f t="shared" si="15"/>
         <v>public string cod_fil_fis  { get; set; }</v>
@@ -22592,7 +22789,7 @@
       </c>
       <c r="J326" s="18" t="str">
         <f t="shared" si="17"/>
-        <v>|if(!string.IsNullOrWhiteSpace(msg.codigoFilialPessoaFisica))| .cod_fil_fis = msg.codigoFilialPessoaFisica;</v>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.codigoFilialPessoaFisica))| registroVinculo.cod_fil_fis = msg.codigoFilialPessoaFisica;</v>
       </c>
     </row>
     <row r="327" spans="1:10" x14ac:dyDescent="0.25">
@@ -22614,6 +22811,9 @@
       <c r="F327" s="22" t="s">
         <v>993</v>
       </c>
+      <c r="G327" s="22" t="s">
+        <v>1114</v>
+      </c>
       <c r="H327" s="18" t="str">
         <f t="shared" si="15"/>
         <v>public int seq_vinculo  { get; set; }</v>
@@ -22624,7 +22824,7 @@
       </c>
       <c r="J327" s="18" t="str">
         <f t="shared" si="17"/>
-        <v>|if(msg.numeroSequencia &gt; 0)| .seq_vinculo = msg.numeroSequencia;</v>
+        <v>|if(msg.numeroSequencia &gt; 0)| registroVinculo.seq_vinculo = msg.numeroSequencia;</v>
       </c>
     </row>
     <row r="328" spans="1:10" x14ac:dyDescent="0.25">
@@ -22646,6 +22846,9 @@
       <c r="F328" s="22" t="s">
         <v>3</v>
       </c>
+      <c r="G328" s="22" t="s">
+        <v>1114</v>
+      </c>
       <c r="H328" s="18" t="str">
         <f t="shared" si="15"/>
         <v>public string idc_partcipacao  { get; set; }</v>
@@ -22656,7 +22859,7 @@
       </c>
       <c r="J328" s="18" t="str">
         <f t="shared" si="17"/>
-        <v>|if(!string.IsNullOrWhiteSpace(msg.indicadorParticipacao))| .idc_partcipacao = msg.indicadorParticipacao;</v>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.indicadorParticipacao))| registroVinculo.idc_partcipacao = msg.indicadorParticipacao;</v>
       </c>
     </row>
     <row r="329" spans="1:10" x14ac:dyDescent="0.25">
@@ -22678,6 +22881,9 @@
       <c r="F329" s="22" t="s">
         <v>991</v>
       </c>
+      <c r="G329" s="22" t="s">
+        <v>1114</v>
+      </c>
       <c r="H329" s="18" t="str">
         <f t="shared" si="15"/>
         <v>public decimal pct_participacao  { get; set; }</v>
@@ -22688,7 +22894,7 @@
       </c>
       <c r="J329" s="18" t="str">
         <f t="shared" si="17"/>
-        <v>|if(msg.percentualParticipacao &gt; 0)| .pct_participacao = msg.percentualParticipacao;</v>
+        <v>|if(msg.percentualParticipacao &gt; 0)| registroVinculo.pct_participacao = msg.percentualParticipacao;</v>
       </c>
     </row>
     <row r="330" spans="1:10" x14ac:dyDescent="0.25">
@@ -22710,6 +22916,9 @@
       <c r="F330" s="22" t="s">
         <v>1089</v>
       </c>
+      <c r="G330" s="22" t="s">
+        <v>1114</v>
+      </c>
       <c r="H330" s="18" t="str">
         <f t="shared" si="15"/>
         <v>public DateTime dat_posse  { get; set; }</v>
@@ -22720,7 +22929,7 @@
       </c>
       <c r="J330" s="18" t="str">
         <f t="shared" si="17"/>
-        <v>|if(msg.dataPosse != DateTime.MinValue)| .dat_posse = msg.dataPosse;</v>
+        <v>|if(msg.dataPosse != DateTime.MinValue)| registroVinculo.dat_posse = msg.dataPosse;</v>
       </c>
     </row>
     <row r="331" spans="1:10" x14ac:dyDescent="0.25">
@@ -22740,6 +22949,9 @@
       <c r="F331" s="22" t="s">
         <v>3</v>
       </c>
+      <c r="G331" s="22" t="s">
+        <v>1114</v>
+      </c>
       <c r="H331" s="18" t="str">
         <f t="shared" si="15"/>
         <v>public string tmp_mandato  { get; set; }</v>
@@ -22750,7 +22962,7 @@
       </c>
       <c r="J331" s="18" t="str">
         <f t="shared" si="17"/>
-        <v>|if(!string.IsNullOrWhiteSpace(msg.tempoMandato))| .tmp_mandato = msg.tempoMandato;</v>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.tempoMandato))| registroVinculo.tmp_mandato = msg.tempoMandato;</v>
       </c>
     </row>
     <row r="332" spans="1:10" x14ac:dyDescent="0.25">
@@ -22772,6 +22984,9 @@
       <c r="F332" s="22" t="s">
         <v>3</v>
       </c>
+      <c r="G332" s="22" t="s">
+        <v>1114</v>
+      </c>
       <c r="H332" s="18" t="str">
         <f t="shared" si="15"/>
         <v>public string des_vinc_fisjur  { get; set; }</v>
@@ -22782,7 +22997,7 @@
       </c>
       <c r="J332" s="18" t="str">
         <f t="shared" si="17"/>
-        <v>|if(!string.IsNullOrWhiteSpace(msg.observacao))| .des_vinc_fisjur = msg.observacao;</v>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.observacao))| registroVinculo.des_vinc_fisjur = msg.observacao;</v>
       </c>
     </row>
     <row r="333" spans="1:10" x14ac:dyDescent="0.25">
@@ -22804,6 +23019,9 @@
       <c r="F333" s="22" t="s">
         <v>1089</v>
       </c>
+      <c r="G333" s="22" t="s">
+        <v>1114</v>
+      </c>
       <c r="H333" s="18" t="str">
         <f t="shared" si="15"/>
         <v>public DateTime dat_cad  { get; set; }</v>
@@ -22814,7 +23032,7 @@
       </c>
       <c r="J333" s="18" t="str">
         <f t="shared" si="17"/>
-        <v>|if(msg.dataCadastro != DateTime.MinValue)| .dat_cad = msg.dataCadastro;</v>
+        <v>|if(msg.dataCadastro != DateTime.MinValue)| registroVinculo.dat_cad = msg.dataCadastro;</v>
       </c>
     </row>
     <row r="334" spans="1:10" x14ac:dyDescent="0.25">
@@ -22836,6 +23054,9 @@
       <c r="F334" s="22" t="s">
         <v>3</v>
       </c>
+      <c r="G334" s="22" t="s">
+        <v>1114</v>
+      </c>
       <c r="H334" s="18" t="str">
         <f t="shared" si="15"/>
         <v>public string usu_atu  { get; set; }</v>
@@ -22846,7 +23067,7 @@
       </c>
       <c r="J334" s="18" t="str">
         <f t="shared" si="17"/>
-        <v>|if(!string.IsNullOrWhiteSpace(msg.usuarioUltimaAtualizacao))| .usu_atu = msg.usuarioUltimaAtualizacao;</v>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.usuarioUltimaAtualizacao))| registroVinculo.usu_atu = msg.usuarioUltimaAtualizacao;</v>
       </c>
     </row>
     <row r="335" spans="1:10" x14ac:dyDescent="0.25">
@@ -22868,6 +23089,9 @@
       <c r="F335" s="22" t="s">
         <v>1089</v>
       </c>
+      <c r="G335" s="22" t="s">
+        <v>1114</v>
+      </c>
       <c r="H335" s="18" t="str">
         <f t="shared" si="15"/>
         <v>public DateTime dat_atu  { get; set; }</v>
@@ -22878,7 +23102,7 @@
       </c>
       <c r="J335" s="18" t="str">
         <f t="shared" si="17"/>
-        <v>|if(msg.dataAtualizacao != DateTime.MinValue)| .dat_atu = msg.dataAtualizacao;</v>
+        <v>|if(msg.dataAtualizacao != DateTime.MinValue)| registroVinculo.dat_atu = msg.dataAtualizacao;</v>
       </c>
     </row>
     <row r="336" spans="1:10" x14ac:dyDescent="0.25">
@@ -22900,6 +23124,9 @@
       <c r="F336" s="22" t="s">
         <v>3</v>
       </c>
+      <c r="G336" s="22" t="s">
+        <v>1114</v>
+      </c>
       <c r="H336" s="18" t="str">
         <f t="shared" si="15"/>
         <v>public string idc_sit  { get; set; }</v>
@@ -22910,7 +23137,7 @@
       </c>
       <c r="J336" s="18" t="str">
         <f t="shared" si="17"/>
-        <v>|if(!string.IsNullOrWhiteSpace(msg.indicadorSituacao))| .idc_sit = msg.indicadorSituacao;</v>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.indicadorSituacao))| registroVinculo.idc_sit = msg.indicadorSituacao;</v>
       </c>
     </row>
     <row r="337" spans="1:10" x14ac:dyDescent="0.25">
@@ -22932,6 +23159,9 @@
       <c r="F337" s="22" t="s">
         <v>1089</v>
       </c>
+      <c r="G337" s="22" t="s">
+        <v>1114</v>
+      </c>
       <c r="H337" s="18" t="str">
         <f t="shared" si="15"/>
         <v>public DateTime dat_sit  { get; set; }</v>
@@ -22942,7 +23172,7 @@
       </c>
       <c r="J337" s="18" t="str">
         <f t="shared" si="17"/>
-        <v>|if(msg.dataSituacao != DateTime.MinValue)| .dat_sit = msg.dataSituacao;</v>
+        <v>|if(msg.dataSituacao != DateTime.MinValue)| registroVinculo.dat_sit = msg.dataSituacao;</v>
       </c>
     </row>
     <row r="338" spans="1:10" x14ac:dyDescent="0.25">
@@ -22964,6 +23194,9 @@
       <c r="F338" s="22" t="s">
         <v>993</v>
       </c>
+      <c r="G338" s="22" t="s">
+        <v>1114</v>
+      </c>
       <c r="H338" s="18" t="str">
         <f t="shared" si="15"/>
         <v>public int cod_cargo  { get; set; }</v>
@@ -22974,7 +23207,7 @@
       </c>
       <c r="J338" s="18" t="str">
         <f t="shared" si="17"/>
-        <v>|if(msg.codigoCargo &gt; 0)| .cod_cargo = msg.codigoCargo;</v>
+        <v>|if(msg.codigoCargo &gt; 0)| registroVinculo.cod_cargo = msg.codigoCargo;</v>
       </c>
     </row>
     <row r="339" spans="1:10" x14ac:dyDescent="0.25">
@@ -22996,6 +23229,9 @@
       <c r="F339" s="22" t="s">
         <v>3</v>
       </c>
+      <c r="G339" s="22" t="s">
+        <v>1114</v>
+      </c>
       <c r="H339" s="18" t="str">
         <f t="shared" si="15"/>
         <v>public string idc_assina  { get; set; }</v>
@@ -23006,7 +23242,7 @@
       </c>
       <c r="J339" s="18" t="str">
         <f t="shared" si="17"/>
-        <v>|if(!string.IsNullOrWhiteSpace(msg.indicadorAssinaEmpresa))| .idc_assina = msg.indicadorAssinaEmpresa;</v>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.indicadorAssinaEmpresa))| registroVinculo.idc_assina = msg.indicadorAssinaEmpresa;</v>
       </c>
     </row>
     <row r="340" spans="1:10" x14ac:dyDescent="0.25">
@@ -23028,6 +23264,9 @@
       <c r="F340" s="22" t="s">
         <v>3</v>
       </c>
+      <c r="G340" s="22" t="s">
+        <v>1114</v>
+      </c>
       <c r="H340" s="18" t="str">
         <f t="shared" si="15"/>
         <v>public string idc_contato  { get; set; }</v>
@@ -23038,7 +23277,7 @@
       </c>
       <c r="J340" s="18" t="str">
         <f t="shared" si="17"/>
-        <v>|if(!string.IsNullOrWhiteSpace(msg.indicadorContato))| .idc_contato = msg.indicadorContato;</v>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.indicadorContato))| registroVinculo.idc_contato = msg.indicadorContato;</v>
       </c>
     </row>
     <row r="341" spans="1:10" x14ac:dyDescent="0.25">
@@ -23060,6 +23299,9 @@
       <c r="F341" s="22" t="s">
         <v>1089</v>
       </c>
+      <c r="G341" s="22" t="s">
+        <v>1114</v>
+      </c>
       <c r="H341" s="18" t="str">
         <f t="shared" si="15"/>
         <v>public DateTime dat_fim  { get; set; }</v>
@@ -23070,7 +23312,7 @@
       </c>
       <c r="J341" s="18" t="str">
         <f t="shared" si="17"/>
-        <v>|if(msg.dataFim != DateTime.MinValue)| .dat_fim = msg.dataFim;</v>
+        <v>|if(msg.dataFim != DateTime.MinValue)| registroVinculo.dat_fim = msg.dataFim;</v>
       </c>
     </row>
     <row r="342" spans="1:10" x14ac:dyDescent="0.25">
@@ -23092,6 +23334,9 @@
       <c r="F342" s="22" t="s">
         <v>3</v>
       </c>
+      <c r="G342" s="22" t="s">
+        <v>1114</v>
+      </c>
       <c r="H342" s="18" t="str">
         <f t="shared" si="15"/>
         <v>public string cod_vinculo  { get; set; }</v>
@@ -23102,7 +23347,7 @@
       </c>
       <c r="J342" s="18" t="str">
         <f t="shared" si="17"/>
-        <v>|if(!string.IsNullOrWhiteSpace(msg.codigoVinculo))| .cod_vinculo = msg.codigoVinculo;</v>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.codigoVinculo))| registroVinculo.cod_vinculo = msg.codigoVinculo;</v>
       </c>
     </row>
     <row r="343" spans="1:10" x14ac:dyDescent="0.25">
@@ -23124,6 +23369,9 @@
       <c r="F343" s="22" t="s">
         <v>1089</v>
       </c>
+      <c r="G343" s="22" t="s">
+        <v>1114</v>
+      </c>
       <c r="H343" s="18" t="str">
         <f t="shared" si="15"/>
         <v>public DateTime dat_venc_proc  { get; set; }</v>
@@ -23134,7 +23382,7 @@
       </c>
       <c r="J343" s="18" t="str">
         <f t="shared" si="17"/>
-        <v>|if(msg.dataVencimentoProcuracao != DateTime.MinValue)| .dat_venc_proc = msg.dataVencimentoProcuracao;</v>
+        <v>|if(msg.dataVencimentoProcuracao != DateTime.MinValue)| registroVinculo.dat_venc_proc = msg.dataVencimentoProcuracao;</v>
       </c>
     </row>
     <row r="344" spans="1:10" x14ac:dyDescent="0.25">
@@ -23154,6 +23402,9 @@
       <c r="F344" s="22" t="s">
         <v>1089</v>
       </c>
+      <c r="G344" s="22" t="s">
+        <v>1114</v>
+      </c>
       <c r="H344" s="18" t="str">
         <f t="shared" si="15"/>
         <v>public DateTime tmp_mandato_1  { get; set; }</v>
@@ -23164,7 +23415,7 @@
       </c>
       <c r="J344" s="18" t="str">
         <f t="shared" si="17"/>
-        <v>|if(msg.tempoMandato1 != DateTime.MinValue)| .tmp_mandato_1 = msg.tempoMandato1;</v>
+        <v>|if(msg.tempoMandato1 != DateTime.MinValue)| registroVinculo.tmp_mandato_1 = msg.tempoMandato1;</v>
       </c>
     </row>
     <row r="345" spans="1:10" x14ac:dyDescent="0.25">
@@ -23186,6 +23437,9 @@
       <c r="F345" s="22" t="s">
         <v>1089</v>
       </c>
+      <c r="G345" s="22" t="s">
+        <v>1114</v>
+      </c>
       <c r="H345" s="18" t="str">
         <f t="shared" si="15"/>
         <v>public DateTime dat_fim_mandato  { get; set; }</v>
@@ -23196,7 +23450,7 @@
       </c>
       <c r="J345" s="18" t="str">
         <f t="shared" si="17"/>
-        <v>|if(msg.dataFimMandato != DateTime.MinValue)| .dat_fim_mandato = msg.dataFimMandato;</v>
+        <v>|if(msg.dataFimMandato != DateTime.MinValue)| registroVinculo.dat_fim_mandato = msg.dataFimMandato;</v>
       </c>
     </row>
     <row r="346" spans="1:10" x14ac:dyDescent="0.25">
@@ -23218,6 +23472,9 @@
       <c r="F346" s="22" t="s">
         <v>3</v>
       </c>
+      <c r="G346" s="22" t="s">
+        <v>1114</v>
+      </c>
       <c r="H346" s="18" t="str">
         <f t="shared" si="15"/>
         <v>public string nom_pessoa  { get; set; }</v>
@@ -23228,7 +23485,7 @@
       </c>
       <c r="J346" s="18" t="str">
         <f t="shared" si="17"/>
-        <v>|if(!string.IsNullOrWhiteSpace(msg.nomePessoa))| .nom_pessoa = msg.nomePessoa;</v>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.nomePessoa))| registroVinculo.nom_pessoa = msg.nomePessoa;</v>
       </c>
     </row>
     <row r="347" spans="1:10" x14ac:dyDescent="0.25">
@@ -23250,6 +23507,9 @@
       <c r="F347" s="18" t="s">
         <v>3</v>
       </c>
+      <c r="G347" s="22" t="s">
+        <v>1114</v>
+      </c>
       <c r="H347" s="18" t="str">
         <f t="shared" si="15"/>
         <v>public string cpf_cnpj_soc  { get; set; }</v>
@@ -23260,7 +23520,7 @@
       </c>
       <c r="J347" s="18" t="str">
         <f t="shared" si="17"/>
-        <v>|if(!string.IsNullOrWhiteSpace(msg.CNPJCPFSoc))| .cpf_cnpj_soc = msg.CNPJCPFSoc;</v>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.CNPJCPFSoc))| registroVinculo.cpf_cnpj_soc = msg.CNPJCPFSoc;</v>
       </c>
     </row>
     <row r="348" spans="1:10" x14ac:dyDescent="0.25">
@@ -23282,6 +23542,9 @@
       <c r="F348" s="22" t="s">
         <v>3</v>
       </c>
+      <c r="G348" s="22" t="s">
+        <v>1114</v>
+      </c>
       <c r="H348" s="18" t="str">
         <f t="shared" si="15"/>
         <v>public string tip_pes_soc  { get; set; }</v>
@@ -23292,7 +23555,7 @@
       </c>
       <c r="J348" s="18" t="str">
         <f t="shared" si="17"/>
-        <v>|if(!string.IsNullOrWhiteSpace(msg.tipoPesoa))| .tip_pes_soc = msg.tipoPesoa;</v>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.tipoPesoa))| registroVinculo.tip_pes_soc = msg.tipoPesoa;</v>
       </c>
     </row>
     <row r="349" spans="1:10" x14ac:dyDescent="0.25">
@@ -23312,6 +23575,9 @@
       <c r="F349" s="19" t="s">
         <v>993</v>
       </c>
+      <c r="G349" s="22" t="s">
+        <v>1114</v>
+      </c>
       <c r="H349" s="18" t="str">
         <f t="shared" si="15"/>
         <v>public int ppsseqpes  { get; set; }</v>
@@ -23322,7 +23588,7 @@
       </c>
       <c r="J349" s="18" t="str">
         <f t="shared" si="17"/>
-        <v>|if(msg.ppsseqpes &gt; 0)| .ppsseqpes = msg.ppsseqpes;</v>
+        <v>|if(msg.ppsseqpes &gt; 0)| registroVinculo.ppsseqpes = msg.ppsseqpes;</v>
       </c>
     </row>
     <row r="350" spans="1:10" x14ac:dyDescent="0.25">
@@ -23342,6 +23608,9 @@
       <c r="F350" s="19" t="s">
         <v>992</v>
       </c>
+      <c r="G350" s="22" t="s">
+        <v>1114</v>
+      </c>
       <c r="H350" s="18" t="str">
         <f t="shared" si="15"/>
         <v>public dateTime pepdthatu  { get; set; }</v>
@@ -23352,7 +23621,7 @@
       </c>
       <c r="J350" s="18" t="str">
         <f t="shared" si="17"/>
-        <v>|if(msg.pepdthatu != DateTime.MinValue)| .pepdthatu = msg.pepdthatu;</v>
+        <v>|if(msg.pepdthatu != DateTime.MinValue)| registroVinculo.pepdthatu = msg.pepdthatu;</v>
       </c>
     </row>
     <row r="351" spans="1:10" x14ac:dyDescent="0.25">
@@ -23372,6 +23641,9 @@
       <c r="F351" s="18" t="s">
         <v>3</v>
       </c>
+      <c r="G351" s="22" t="s">
+        <v>1114</v>
+      </c>
       <c r="H351" s="18" t="str">
         <f t="shared" si="15"/>
         <v>public string pepidcpep  { get; set; }</v>
@@ -23382,7 +23654,7 @@
       </c>
       <c r="J351" s="18" t="str">
         <f t="shared" si="17"/>
-        <v>|if(!string.IsNullOrWhiteSpace(msg.pepidcpep))| .pepidcpep = msg.pepidcpep;</v>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.pepidcpep))| registroVinculo.pepidcpep = msg.pepidcpep;</v>
       </c>
     </row>
     <row r="352" spans="1:10" x14ac:dyDescent="0.25">
@@ -23404,6 +23676,9 @@
       <c r="F352" s="21" t="s">
         <v>3</v>
       </c>
+      <c r="G352" s="22" t="s">
+        <v>1114</v>
+      </c>
       <c r="H352" s="18" t="str">
         <f t="shared" si="15"/>
         <v>public string idc_emite_dupl  { get; set; }</v>
@@ -23414,7 +23689,7 @@
       </c>
       <c r="J352" s="18" t="str">
         <f t="shared" si="17"/>
-        <v>|if(!string.IsNullOrWhiteSpace(msg.indicadorEmiteDuplicata))| .idc_emite_dupl = msg.indicadorEmiteDuplicata;</v>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.indicadorEmiteDuplicata))| registroVinculo.idc_emite_dupl = msg.indicadorEmiteDuplicata;</v>
       </c>
     </row>
     <row r="353" spans="1:10" x14ac:dyDescent="0.25">
@@ -23436,6 +23711,9 @@
       <c r="F353" s="21" t="s">
         <v>3</v>
       </c>
+      <c r="G353" s="22" t="s">
+        <v>1114</v>
+      </c>
       <c r="H353" s="18" t="str">
         <f t="shared" si="15"/>
         <v>public string idc_assina_endosso  { get; set; }</v>
@@ -23446,7 +23724,7 @@
       </c>
       <c r="J353" s="18" t="str">
         <f t="shared" si="17"/>
-        <v>|if(!string.IsNullOrWhiteSpace(msg.indicadorAssinaEndosso))| .idc_assina_endosso = msg.indicadorAssinaEndosso;</v>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.indicadorAssinaEndosso))| registroVinculo.idc_assina_endosso = msg.indicadorAssinaEndosso;</v>
       </c>
     </row>
     <row r="354" spans="1:10" x14ac:dyDescent="0.25">
@@ -23468,6 +23746,9 @@
       <c r="F354" s="21" t="s">
         <v>3</v>
       </c>
+      <c r="G354" s="22" t="s">
+        <v>1114</v>
+      </c>
       <c r="H354" s="18" t="str">
         <f t="shared" si="15"/>
         <v>public string idc_assina_cessao  { get; set; }</v>
@@ -23478,7 +23759,7 @@
       </c>
       <c r="J354" s="18" t="str">
         <f t="shared" si="17"/>
-        <v>|if(!string.IsNullOrWhiteSpace(msg.indicadorAssinaCessao))| .idc_assina_cessao = msg.indicadorAssinaCessao;</v>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.indicadorAssinaCessao))| registroVinculo.idc_assina_cessao = msg.indicadorAssinaCessao;</v>
       </c>
     </row>
     <row r="355" spans="1:10" x14ac:dyDescent="0.25">
@@ -23500,6 +23781,9 @@
       <c r="F355" s="21" t="s">
         <v>3</v>
       </c>
+      <c r="G355" s="22" t="s">
+        <v>1114</v>
+      </c>
       <c r="H355" s="18" t="str">
         <f t="shared" si="15"/>
         <v>public string idc_assina_isoladamente  { get; set; }</v>
@@ -23510,7 +23794,7 @@
       </c>
       <c r="J355" s="18" t="str">
         <f t="shared" si="17"/>
-        <v>|if(!string.IsNullOrWhiteSpace(msg.indicadorAssinaIsoladamente))| .idc_assina_isoladamente = msg.indicadorAssinaIsoladamente;</v>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.indicadorAssinaIsoladamente))| registroVinculo.idc_assina_isoladamente = msg.indicadorAssinaIsoladamente;</v>
       </c>
     </row>
     <row r="356" spans="1:10" x14ac:dyDescent="0.25">
@@ -23532,6 +23816,9 @@
       <c r="F356" s="21" t="s">
         <v>3</v>
       </c>
+      <c r="G356" s="22" t="s">
+        <v>1114</v>
+      </c>
       <c r="H356" s="18" t="str">
         <f t="shared" ref="H356:H362" si="18">CONCATENATE("public ",F356," ",B356,"  { get; set; }")</f>
         <v>public string cod_pessoa_assina1  { get; set; }</v>
@@ -23542,7 +23829,7 @@
       </c>
       <c r="J356" s="18" t="str">
         <f t="shared" si="17"/>
-        <v>|if(!string.IsNullOrWhiteSpace(msg.codigoPessoaAssina1))| .cod_pessoa_assina1 = msg.codigoPessoaAssina1;</v>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.codigoPessoaAssina1))| registroVinculo.cod_pessoa_assina1 = msg.codigoPessoaAssina1;</v>
       </c>
     </row>
     <row r="357" spans="1:10" x14ac:dyDescent="0.25">
@@ -23564,6 +23851,9 @@
       <c r="F357" s="21" t="s">
         <v>3</v>
       </c>
+      <c r="G357" s="22" t="s">
+        <v>1114</v>
+      </c>
       <c r="H357" s="18" t="str">
         <f t="shared" si="18"/>
         <v>public string cod_pessoa_assina2  { get; set; }</v>
@@ -23574,7 +23864,7 @@
       </c>
       <c r="J357" s="18" t="str">
         <f t="shared" si="17"/>
-        <v>|if(!string.IsNullOrWhiteSpace(msg.codigoPessoaAssina2))| .cod_pessoa_assina2 = msg.codigoPessoaAssina2;</v>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.codigoPessoaAssina2))| registroVinculo.cod_pessoa_assina2 = msg.codigoPessoaAssina2;</v>
       </c>
     </row>
     <row r="358" spans="1:10" x14ac:dyDescent="0.25">
@@ -23596,6 +23886,9 @@
       <c r="F358" s="21" t="s">
         <v>3</v>
       </c>
+      <c r="G358" s="22" t="s">
+        <v>1114</v>
+      </c>
       <c r="H358" s="18" t="str">
         <f t="shared" si="18"/>
         <v>public string cod_pessoa_assina3  { get; set; }</v>
@@ -23606,7 +23899,7 @@
       </c>
       <c r="J358" s="18" t="str">
         <f t="shared" si="17"/>
-        <v>|if(!string.IsNullOrWhiteSpace(msg.codigoPessoaAssina3))| .cod_pessoa_assina3 = msg.codigoPessoaAssina3;</v>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.codigoPessoaAssina3))| registroVinculo.cod_pessoa_assina3 = msg.codigoPessoaAssina3;</v>
       </c>
     </row>
     <row r="359" spans="1:10" x14ac:dyDescent="0.25">
@@ -23628,6 +23921,9 @@
       <c r="F359" s="18" t="s">
         <v>3</v>
       </c>
+      <c r="G359" s="22" t="s">
+        <v>1114</v>
+      </c>
       <c r="H359" s="18" t="str">
         <f t="shared" si="18"/>
         <v>public string nom_assina1  { get; set; }</v>
@@ -23638,7 +23934,7 @@
       </c>
       <c r="J359" s="18" t="str">
         <f t="shared" si="17"/>
-        <v>|if(!string.IsNullOrWhiteSpace(msg.nomeAssina1))| .nom_assina1 = msg.nomeAssina1;</v>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.nomeAssina1))| registroVinculo.nom_assina1 = msg.nomeAssina1;</v>
       </c>
     </row>
     <row r="360" spans="1:10" x14ac:dyDescent="0.25">
@@ -23660,6 +23956,9 @@
       <c r="F360" s="18" t="s">
         <v>3</v>
       </c>
+      <c r="G360" s="22" t="s">
+        <v>1114</v>
+      </c>
       <c r="H360" s="18" t="str">
         <f t="shared" si="18"/>
         <v>public string nom_assina2  { get; set; }</v>
@@ -23670,7 +23969,7 @@
       </c>
       <c r="J360" s="18" t="str">
         <f t="shared" si="17"/>
-        <v>|if(!string.IsNullOrWhiteSpace(msg.nomeAssina2))| .nom_assina2 = msg.nomeAssina2;</v>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.nomeAssina2))| registroVinculo.nom_assina2 = msg.nomeAssina2;</v>
       </c>
     </row>
     <row r="361" spans="1:10" x14ac:dyDescent="0.25">
@@ -23692,6 +23991,9 @@
       <c r="F361" s="18" t="s">
         <v>3</v>
       </c>
+      <c r="G361" s="22" t="s">
+        <v>1114</v>
+      </c>
       <c r="H361" s="18" t="str">
         <f t="shared" si="18"/>
         <v>public string nom_assina3  { get; set; }</v>
@@ -23702,7 +24004,7 @@
       </c>
       <c r="J361" s="18" t="str">
         <f t="shared" si="17"/>
-        <v>|if(!string.IsNullOrWhiteSpace(msg.nomeAssina3))| .nom_assina3 = msg.nomeAssina3;</v>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.nomeAssina3))| registroVinculo.nom_assina3 = msg.nomeAssina3;</v>
       </c>
     </row>
     <row r="362" spans="1:10" x14ac:dyDescent="0.25">
@@ -23722,6 +24024,9 @@
       <c r="F362" s="21" t="s">
         <v>3</v>
       </c>
+      <c r="G362" s="22" t="s">
+        <v>1114</v>
+      </c>
       <c r="H362" s="18" t="str">
         <f t="shared" si="18"/>
         <v>public string fisjuremailvinculo  { get; set; }</v>
@@ -23732,7 +24037,7 @@
       </c>
       <c r="J362" s="18" t="str">
         <f t="shared" si="17"/>
-        <v>|if(!string.IsNullOrWhiteSpace(msg.emailVinculo))| .fisjuremailvinculo = msg.emailVinculo;</v>
+        <v>|if(!string.IsNullOrWhiteSpace(msg.emailVinculo))| registroVinculo.fisjuremailvinculo = msg.emailVinculo;</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Inclusão no excel gerador do serviços
</commit_message>
<xml_diff>
--- a/API/documentos/Dados Entrada Cliente.xlsx
+++ b/API/documentos/Dados Entrada Cliente.xlsx
@@ -16,6 +16,7 @@
     <sheet name="Geração adaptador" sheetId="4" r:id="rId2"/>
     <sheet name="geração json" sheetId="2" r:id="rId3"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8094" uniqueCount="1123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8214" uniqueCount="1158">
   <si>
     <t>tb_pes</t>
   </si>
@@ -3396,6 +3397,111 @@
   </si>
   <si>
     <t>classeMsg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cod_fil </t>
+  </si>
+  <si>
+    <t>COD_CTA_RESGATE</t>
+  </si>
+  <si>
+    <t>NEGIDCBCO</t>
+  </si>
+  <si>
+    <t>NEGCODISPB</t>
+  </si>
+  <si>
+    <t>IPGCOD</t>
+  </si>
+  <si>
+    <t>NEGSTACONTAPADRAO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Código de pessoa </t>
+  </si>
+  <si>
+    <t>Código de filial</t>
+  </si>
+  <si>
+    <t>Sequencial negócio</t>
+  </si>
+  <si>
+    <t>Código da agência</t>
+  </si>
+  <si>
+    <t>Número da conta</t>
+  </si>
+  <si>
+    <t>Valor do limite</t>
+  </si>
+  <si>
+    <t>Saldo devedor</t>
+  </si>
+  <si>
+    <t>Data de inicio da operação</t>
+  </si>
+  <si>
+    <t>Data de fim da operação</t>
+  </si>
+  <si>
+    <t>Data de cadastramento</t>
+  </si>
+  <si>
+    <t>Último usuário de atualização</t>
+  </si>
+  <si>
+    <t>Data da última atualização</t>
+  </si>
+  <si>
+    <t>Data da situação</t>
+  </si>
+  <si>
+    <t>Identificador de situação</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Código Empresa </t>
+  </si>
+  <si>
+    <t>Código do produto bancário</t>
+  </si>
+  <si>
+    <t>Código do Banco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Código do banco do negócio </t>
+  </si>
+  <si>
+    <t>Conta de Crédito para Resgate</t>
+  </si>
+  <si>
+    <t>Situação do Registro</t>
+  </si>
+  <si>
+    <t>Indica se é Banco ou Instituição de Pagamento</t>
+  </si>
+  <si>
+    <t>Código ISPB do banco</t>
+  </si>
+  <si>
+    <t>Código de Instituição de Pagamento</t>
+  </si>
+  <si>
+    <t>Indica se é Conta Padrão ou não - S - sim | N - não</t>
+  </si>
+  <si>
+    <t>valdoDevedor</t>
+  </si>
+  <si>
+    <t>identificadorSituacao</t>
+  </si>
+  <si>
+    <t>SituacaoRegistro</t>
+  </si>
+  <si>
+    <t>IndicadorBancoOuInstPagamento</t>
+  </si>
+  <si>
+    <t>codigoInstPagamento</t>
   </si>
 </sst>
 </file>
@@ -3832,10 +3938,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G362"/>
+  <dimension ref="A1:G387"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A266" workbookViewId="0">
-      <selection activeCell="A278" sqref="A278"/>
+    <sheetView tabSelected="1" topLeftCell="B241" workbookViewId="0">
+      <selection activeCell="E260" sqref="E260"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10977,7 +11083,7 @@
         <v>3</v>
       </c>
       <c r="G324" s="14" t="str">
-        <f t="shared" ref="G324:G362" si="5">CONCATENATE("|/// &lt;summary&gt;|/// ",D324,"|/// &lt;/summary&gt;| public ",F324," ",E324," { get; set; }")</f>
+        <f t="shared" ref="G324:G386" si="5">CONCATENATE("|/// &lt;summary&gt;|/// ",D324,"|/// &lt;/summary&gt;| public ",F324," ",E324," { get; set; }")</f>
         <v>|/// &lt;summary&gt;|/// Filial|/// &lt;/summary&gt;| public string codigoFilialPessoaJuridica { get; set; }</v>
       </c>
     </row>
@@ -11804,6 +11910,537 @@
         <f t="shared" si="5"/>
         <v>|/// &lt;summary&gt;|/// |/// &lt;/summary&gt;| public string emailVinculo { get; set; }</v>
       </c>
+    </row>
+    <row r="363" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A363" s="20" t="s">
+        <v>580</v>
+      </c>
+      <c r="B363" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C363" s="20"/>
+      <c r="D363" s="20" t="s">
+        <v>1129</v>
+      </c>
+      <c r="E363" s="20" t="s">
+        <v>630</v>
+      </c>
+      <c r="F363" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="G363" s="18" t="str">
+        <f t="shared" si="5"/>
+        <v>|/// &lt;summary&gt;|/// Código de pessoa |/// &lt;/summary&gt;| public string codigoPessoa { get; set; }</v>
+      </c>
+    </row>
+    <row r="364" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A364" s="20" t="s">
+        <v>580</v>
+      </c>
+      <c r="B364" s="20" t="s">
+        <v>1123</v>
+      </c>
+      <c r="C364" s="20"/>
+      <c r="D364" s="20" t="s">
+        <v>1130</v>
+      </c>
+      <c r="E364" s="20" t="s">
+        <v>680</v>
+      </c>
+      <c r="F364" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="G364" s="18" t="str">
+        <f t="shared" si="5"/>
+        <v>|/// &lt;summary&gt;|/// Código de filial|/// &lt;/summary&gt;| public string codigoFilial { get; set; }</v>
+      </c>
+    </row>
+    <row r="365" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A365" s="20" t="s">
+        <v>580</v>
+      </c>
+      <c r="B365" s="20" t="s">
+        <v>581</v>
+      </c>
+      <c r="C365" s="20"/>
+      <c r="D365" s="20" t="s">
+        <v>1131</v>
+      </c>
+      <c r="E365" s="20" t="s">
+        <v>854</v>
+      </c>
+      <c r="F365" s="20" t="s">
+        <v>993</v>
+      </c>
+      <c r="G365" s="18" t="str">
+        <f t="shared" si="5"/>
+        <v>|/// &lt;summary&gt;|/// Sequencial negócio|/// &lt;/summary&gt;| public int sequencial { get; set; }</v>
+      </c>
+    </row>
+    <row r="366" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A366" s="20" t="s">
+        <v>580</v>
+      </c>
+      <c r="B366" s="20" t="s">
+        <v>582</v>
+      </c>
+      <c r="C366" s="20"/>
+      <c r="D366" s="20" t="s">
+        <v>1132</v>
+      </c>
+      <c r="E366" s="20" t="s">
+        <v>921</v>
+      </c>
+      <c r="F366" s="20" t="s">
+        <v>993</v>
+      </c>
+      <c r="G366" s="18" t="str">
+        <f t="shared" si="5"/>
+        <v>|/// &lt;summary&gt;|/// Código da agência|/// &lt;/summary&gt;| public int codigoAgencia { get; set; }</v>
+      </c>
+    </row>
+    <row r="367" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A367" s="20" t="s">
+        <v>580</v>
+      </c>
+      <c r="B367" s="20" t="s">
+        <v>583</v>
+      </c>
+      <c r="C367" s="20"/>
+      <c r="D367" s="20" t="s">
+        <v>1133</v>
+      </c>
+      <c r="E367" s="20" t="s">
+        <v>922</v>
+      </c>
+      <c r="F367" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="G367" s="18" t="str">
+        <f t="shared" si="5"/>
+        <v>|/// &lt;summary&gt;|/// Número da conta|/// &lt;/summary&gt;| public string numeroConta { get; set; }</v>
+      </c>
+    </row>
+    <row r="368" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A368" s="20" t="s">
+        <v>580</v>
+      </c>
+      <c r="B368" s="20" t="s">
+        <v>584</v>
+      </c>
+      <c r="C368" s="20"/>
+      <c r="D368" s="20" t="s">
+        <v>1134</v>
+      </c>
+      <c r="E368" s="20" t="s">
+        <v>863</v>
+      </c>
+      <c r="F368" s="20" t="s">
+        <v>991</v>
+      </c>
+      <c r="G368" s="18" t="str">
+        <f t="shared" si="5"/>
+        <v>|/// &lt;summary&gt;|/// Valor do limite|/// &lt;/summary&gt;| public decimal valorLimite { get; set; }</v>
+      </c>
+    </row>
+    <row r="369" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A369" s="20" t="s">
+        <v>580</v>
+      </c>
+      <c r="B369" s="20" t="s">
+        <v>585</v>
+      </c>
+      <c r="C369" s="20"/>
+      <c r="D369" s="20" t="s">
+        <v>1135</v>
+      </c>
+      <c r="E369" s="20" t="s">
+        <v>1153</v>
+      </c>
+      <c r="F369" s="20" t="s">
+        <v>991</v>
+      </c>
+      <c r="G369" s="18" t="str">
+        <f t="shared" si="5"/>
+        <v>|/// &lt;summary&gt;|/// Saldo devedor|/// &lt;/summary&gt;| public decimal valdoDevedor { get; set; }</v>
+      </c>
+    </row>
+    <row r="370" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A370" s="20" t="s">
+        <v>580</v>
+      </c>
+      <c r="B370" s="20" t="s">
+        <v>586</v>
+      </c>
+      <c r="C370" s="20"/>
+      <c r="D370" s="20" t="s">
+        <v>1136</v>
+      </c>
+      <c r="E370" s="20" t="s">
+        <v>717</v>
+      </c>
+      <c r="F370" s="20" t="s">
+        <v>1089</v>
+      </c>
+      <c r="G370" s="18" t="str">
+        <f t="shared" si="5"/>
+        <v>|/// &lt;summary&gt;|/// Data de inicio da operação|/// &lt;/summary&gt;| public DateTime dataInicio { get; set; }</v>
+      </c>
+    </row>
+    <row r="371" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A371" s="20" t="s">
+        <v>580</v>
+      </c>
+      <c r="B371" s="20" t="s">
+        <v>587</v>
+      </c>
+      <c r="C371" s="20"/>
+      <c r="D371" s="20" t="s">
+        <v>1137</v>
+      </c>
+      <c r="E371" s="20" t="s">
+        <v>718</v>
+      </c>
+      <c r="F371" s="20" t="s">
+        <v>1089</v>
+      </c>
+      <c r="G371" s="18" t="str">
+        <f t="shared" si="5"/>
+        <v>|/// &lt;summary&gt;|/// Data de fim da operação|/// &lt;/summary&gt;| public DateTime dataFim { get; set; }</v>
+      </c>
+    </row>
+    <row r="372" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A372" s="20" t="s">
+        <v>580</v>
+      </c>
+      <c r="B372" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="C372" s="20"/>
+      <c r="D372" s="20" t="s">
+        <v>1138</v>
+      </c>
+      <c r="E372" s="20" t="s">
+        <v>642</v>
+      </c>
+      <c r="F372" s="20" t="s">
+        <v>1089</v>
+      </c>
+      <c r="G372" s="18" t="str">
+        <f t="shared" si="5"/>
+        <v>|/// &lt;summary&gt;|/// Data de cadastramento|/// &lt;/summary&gt;| public DateTime dataCadastro { get; set; }</v>
+      </c>
+    </row>
+    <row r="373" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A373" s="20" t="s">
+        <v>580</v>
+      </c>
+      <c r="B373" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C373" s="20"/>
+      <c r="D373" s="20" t="s">
+        <v>1139</v>
+      </c>
+      <c r="E373" s="20" t="s">
+        <v>765</v>
+      </c>
+      <c r="F373" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="G373" s="18" t="str">
+        <f t="shared" si="5"/>
+        <v>|/// &lt;summary&gt;|/// Último usuário de atualização|/// &lt;/summary&gt;| public string usuarioUltimaAtualizacao { get; set; }</v>
+      </c>
+    </row>
+    <row r="374" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A374" s="20" t="s">
+        <v>580</v>
+      </c>
+      <c r="B374" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C374" s="20"/>
+      <c r="D374" s="20" t="s">
+        <v>1140</v>
+      </c>
+      <c r="E374" s="20" t="s">
+        <v>644</v>
+      </c>
+      <c r="F374" s="20" t="s">
+        <v>1089</v>
+      </c>
+      <c r="G374" s="18" t="str">
+        <f t="shared" si="5"/>
+        <v>|/// &lt;summary&gt;|/// Data da última atualização|/// &lt;/summary&gt;| public DateTime dataAtualizacao { get; set; }</v>
+      </c>
+    </row>
+    <row r="375" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A375" s="20" t="s">
+        <v>580</v>
+      </c>
+      <c r="B375" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="C375" s="20"/>
+      <c r="D375" s="20" t="s">
+        <v>1141</v>
+      </c>
+      <c r="E375" s="20" t="s">
+        <v>767</v>
+      </c>
+      <c r="F375" s="20" t="s">
+        <v>1089</v>
+      </c>
+      <c r="G375" s="18" t="str">
+        <f t="shared" si="5"/>
+        <v>|/// &lt;summary&gt;|/// Data da situação|/// &lt;/summary&gt;| public DateTime dataSituacao { get; set; }</v>
+      </c>
+    </row>
+    <row r="376" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A376" s="20" t="s">
+        <v>580</v>
+      </c>
+      <c r="B376" s="20" t="s">
+        <v>313</v>
+      </c>
+      <c r="C376" s="20"/>
+      <c r="D376" s="20" t="s">
+        <v>1142</v>
+      </c>
+      <c r="E376" s="20" t="s">
+        <v>1154</v>
+      </c>
+      <c r="F376" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="G376" s="18" t="str">
+        <f t="shared" si="5"/>
+        <v>|/// &lt;summary&gt;|/// Identificador de situação|/// &lt;/summary&gt;| public string identificadorSituacao { get; set; }</v>
+      </c>
+    </row>
+    <row r="377" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A377" s="20" t="s">
+        <v>580</v>
+      </c>
+      <c r="B377" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="C377" s="20"/>
+      <c r="D377" s="20" t="s">
+        <v>1143</v>
+      </c>
+      <c r="E377" s="20" t="s">
+        <v>692</v>
+      </c>
+      <c r="F377" s="20" t="s">
+        <v>993</v>
+      </c>
+      <c r="G377" s="18" t="str">
+        <f t="shared" si="5"/>
+        <v>|/// &lt;summary&gt;|/// Código Empresa |/// &lt;/summary&gt;| public int codigoEmpresa { get; set; }</v>
+      </c>
+    </row>
+    <row r="378" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A378" s="20" t="s">
+        <v>580</v>
+      </c>
+      <c r="B378" s="20" t="s">
+        <v>588</v>
+      </c>
+      <c r="C378" s="20"/>
+      <c r="D378" s="20" t="s">
+        <v>1144</v>
+      </c>
+      <c r="E378" s="20" t="s">
+        <v>925</v>
+      </c>
+      <c r="F378" s="20" t="s">
+        <v>993</v>
+      </c>
+      <c r="G378" s="18" t="str">
+        <f t="shared" si="5"/>
+        <v>|/// &lt;summary&gt;|/// Código do produto bancário|/// &lt;/summary&gt;| public int codigoProdutoBancario { get; set; }</v>
+      </c>
+    </row>
+    <row r="379" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A379" s="20" t="s">
+        <v>580</v>
+      </c>
+      <c r="B379" s="20" t="s">
+        <v>589</v>
+      </c>
+      <c r="C379" s="20"/>
+      <c r="D379" s="20" t="s">
+        <v>1145</v>
+      </c>
+      <c r="E379" s="20" t="s">
+        <v>926</v>
+      </c>
+      <c r="F379" s="20" t="s">
+        <v>993</v>
+      </c>
+      <c r="G379" s="18" t="str">
+        <f t="shared" si="5"/>
+        <v>|/// &lt;summary&gt;|/// Código do Banco|/// &lt;/summary&gt;| public int codigoBanco { get; set; }</v>
+      </c>
+    </row>
+    <row r="380" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A380" s="20" t="s">
+        <v>580</v>
+      </c>
+      <c r="B380" s="20" t="s">
+        <v>590</v>
+      </c>
+      <c r="C380" s="20"/>
+      <c r="D380" s="20" t="s">
+        <v>1146</v>
+      </c>
+      <c r="E380" s="20" t="s">
+        <v>927</v>
+      </c>
+      <c r="F380" s="20" t="s">
+        <v>993</v>
+      </c>
+      <c r="G380" s="18" t="str">
+        <f t="shared" si="5"/>
+        <v>|/// &lt;summary&gt;|/// Código do banco do negócio |/// &lt;/summary&gt;| public int codigoBancoNegocio { get; set; }</v>
+      </c>
+    </row>
+    <row r="381" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A381" s="20" t="s">
+        <v>580</v>
+      </c>
+      <c r="B381" s="20" t="s">
+        <v>1124</v>
+      </c>
+      <c r="C381" s="20"/>
+      <c r="D381" s="20" t="s">
+        <v>1147</v>
+      </c>
+      <c r="E381" s="20" t="s">
+        <v>929</v>
+      </c>
+      <c r="F381" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="G381" s="18" t="str">
+        <f t="shared" si="5"/>
+        <v>|/// &lt;summary&gt;|/// Conta de Crédito para Resgate|/// &lt;/summary&gt;| public string contaCreditoResgate { get; set; }</v>
+      </c>
+    </row>
+    <row r="382" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A382" s="20" t="s">
+        <v>580</v>
+      </c>
+      <c r="B382" s="20" t="s">
+        <v>194</v>
+      </c>
+      <c r="C382" s="20"/>
+      <c r="D382" s="20" t="s">
+        <v>1148</v>
+      </c>
+      <c r="E382" s="20" t="s">
+        <v>1155</v>
+      </c>
+      <c r="F382" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="G382" s="18" t="str">
+        <f t="shared" si="5"/>
+        <v>|/// &lt;summary&gt;|/// Situação do Registro|/// &lt;/summary&gt;| public string SituacaoRegistro { get; set; }</v>
+      </c>
+    </row>
+    <row r="383" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A383" s="20" t="s">
+        <v>580</v>
+      </c>
+      <c r="B383" s="20" t="s">
+        <v>1125</v>
+      </c>
+      <c r="C383" s="20"/>
+      <c r="D383" s="20" t="s">
+        <v>1149</v>
+      </c>
+      <c r="E383" s="20" t="s">
+        <v>1156</v>
+      </c>
+      <c r="F383" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="G383" s="18" t="str">
+        <f t="shared" si="5"/>
+        <v>|/// &lt;summary&gt;|/// Indica se é Banco ou Instituição de Pagamento|/// &lt;/summary&gt;| public string IndicadorBancoOuInstPagamento { get; set; }</v>
+      </c>
+    </row>
+    <row r="384" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A384" s="20" t="s">
+        <v>580</v>
+      </c>
+      <c r="B384" s="20" t="s">
+        <v>1126</v>
+      </c>
+      <c r="C384" s="20"/>
+      <c r="D384" s="20" t="s">
+        <v>1150</v>
+      </c>
+      <c r="E384" s="20" t="s">
+        <v>1071</v>
+      </c>
+      <c r="F384" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="G384" s="18" t="str">
+        <f t="shared" si="5"/>
+        <v>|/// &lt;summary&gt;|/// Código ISPB do banco|/// &lt;/summary&gt;| public string codigoIspb { get; set; }</v>
+      </c>
+    </row>
+    <row r="385" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A385" s="20" t="s">
+        <v>580</v>
+      </c>
+      <c r="B385" s="20" t="s">
+        <v>1127</v>
+      </c>
+      <c r="C385" s="20"/>
+      <c r="D385" s="20" t="s">
+        <v>1151</v>
+      </c>
+      <c r="E385" s="20" t="s">
+        <v>1157</v>
+      </c>
+      <c r="F385" s="20" t="s">
+        <v>991</v>
+      </c>
+      <c r="G385" s="18" t="str">
+        <f t="shared" si="5"/>
+        <v>|/// &lt;summary&gt;|/// Código de Instituição de Pagamento|/// &lt;/summary&gt;| public decimal codigoInstPagamento { get; set; }</v>
+      </c>
+    </row>
+    <row r="386" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A386" s="20" t="s">
+        <v>580</v>
+      </c>
+      <c r="B386" s="20" t="s">
+        <v>1128</v>
+      </c>
+      <c r="C386" s="20"/>
+      <c r="D386" s="20" t="s">
+        <v>1152</v>
+      </c>
+      <c r="E386" s="20" t="s">
+        <v>932</v>
+      </c>
+      <c r="F386" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="G386" s="18" t="str">
+        <f t="shared" si="5"/>
+        <v>|/// &lt;summary&gt;|/// Indica se é Conta Padrão ou não - S - sim | N - não|/// &lt;/summary&gt;| public string indicadorContaPadrao { get; set; }</v>
+      </c>
+    </row>
+    <row r="387" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A387" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -45052,4 +45689,16 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>